<commit_message>
first full draft of tiered_seeding.tex
</commit_message>
<xml_diff>
--- a/thesis-tex/images/Brackets/Brackets.xlsx
+++ b/thesis-tex/images/Brackets/Brackets.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leofr\Documents\LeoWork\School\04College\17Senior\thesis\thesis-tex\images\Brackets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B17F46F-B4AA-4BDC-B7AC-C31F2543DF6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62D599C9-4C05-4B6F-82C8-3D7C5D2A9B51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="9" activeTab="18" xr2:uid="{503DA620-194E-433E-B5EB-5393E7537419}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="9" activeTab="17" xr2:uid="{503DA620-194E-433E-B5EB-5393E7537419}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="115">
   <si>
     <t>Georgia</t>
   </si>
@@ -381,6 +381,24 @@
   </si>
   <si>
     <t>Argentina</t>
+  </si>
+  <si>
+    <t>Tier 1</t>
+  </si>
+  <si>
+    <t>Tier 2</t>
+  </si>
+  <si>
+    <t>Tier 4</t>
+  </si>
+  <si>
+    <t>Tier 3</t>
+  </si>
+  <si>
+    <t>Tier 5</t>
+  </si>
+  <si>
+    <t>Tier 6</t>
   </si>
 </sst>
 </file>
@@ -455,7 +473,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="30">
+  <borders count="31">
     <border>
       <left/>
       <right/>
@@ -832,11 +850,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -953,7 +982,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -962,13 +994,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -977,6 +1006,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3183,7 +3217,7 @@
     </row>
     <row r="10" spans="3:7" ht="7.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C10" s="1"/>
-      <c r="D10" s="75" t="s">
+      <c r="D10" s="76" t="s">
         <v>49</v>
       </c>
       <c r="E10" s="1"/>
@@ -3192,7 +3226,7 @@
     </row>
     <row r="11" spans="3:7" ht="7.8" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C11" s="64"/>
-      <c r="D11" s="76"/>
+      <c r="D11" s="77"/>
       <c r="E11" s="1"/>
       <c r="F11" s="20"/>
       <c r="G11" s="1"/>
@@ -3238,7 +3272,7 @@
     </row>
     <row r="17" spans="3:7" ht="7.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C17" s="1"/>
-      <c r="D17" s="75" t="s">
+      <c r="D17" s="76" t="s">
         <v>53</v>
       </c>
       <c r="E17" s="1"/>
@@ -3247,7 +3281,7 @@
     </row>
     <row r="18" spans="3:7" ht="7.8" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C18" s="64"/>
-      <c r="D18" s="76"/>
+      <c r="D18" s="77"/>
       <c r="E18" s="1"/>
       <c r="F18" s="20"/>
       <c r="G18" s="1"/>
@@ -4836,94 +4870,1071 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7C06664-9D9D-4861-B1E9-94FF6B95C706}">
-  <dimension ref="C4:J6"/>
+  <dimension ref="B1:AC37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P17" sqref="P17"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="Y17" sqref="Y17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="10" width="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" style="19" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" style="19" customWidth="1"/>
+    <col min="7" max="10" width="13.6640625" customWidth="1"/>
+    <col min="12" max="12" width="13.6640625" customWidth="1"/>
+    <col min="13" max="13" width="13.6640625" style="19" customWidth="1"/>
+    <col min="14" max="14" width="13.6640625" customWidth="1"/>
+    <col min="15" max="15" width="13.6640625" style="19" customWidth="1"/>
+    <col min="16" max="19" width="13.6640625" customWidth="1"/>
+    <col min="21" max="21" width="13.6640625" customWidth="1"/>
+    <col min="22" max="22" width="13.6640625" style="19" customWidth="1"/>
+    <col min="23" max="23" width="13.6640625" customWidth="1"/>
+    <col min="24" max="24" width="13.6640625" style="19" customWidth="1"/>
+    <col min="25" max="28" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4">
+    <row r="1" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="B1">
+        <v>8</v>
+      </c>
+      <c r="C1">
+        <v>6</v>
+      </c>
+      <c r="D1" s="19">
+        <v>3</v>
+      </c>
+      <c r="L1">
+        <v>6</v>
+      </c>
+      <c r="M1" s="19">
+        <v>3</v>
+      </c>
+      <c r="U1">
+        <v>6</v>
+      </c>
+      <c r="V1" s="19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="C4" s="1"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="6"/>
+      <c r="S4" s="1"/>
+      <c r="U4" s="1"/>
+      <c r="V4" s="6"/>
+      <c r="W4" s="6"/>
+      <c r="X4" s="6"/>
+      <c r="Y4" s="6"/>
+      <c r="Z4" s="1"/>
+      <c r="AA4" s="6"/>
+      <c r="AB4" s="1"/>
+      <c r="AC4" s="1"/>
+    </row>
+    <row r="5" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="C5" s="1"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="6"/>
+      <c r="S5" s="1"/>
+      <c r="U5" s="1"/>
+      <c r="V5" s="6"/>
+      <c r="W5" s="1"/>
+      <c r="X5" s="6"/>
+      <c r="Y5" s="1"/>
+      <c r="Z5" s="1"/>
+      <c r="AA5" s="6"/>
+      <c r="AB5" s="1"/>
+      <c r="AC5" s="1"/>
+    </row>
+    <row r="6" spans="2:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C6" s="1"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="82"/>
+      <c r="F6" s="6">
+        <v>1</v>
+      </c>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="82"/>
+      <c r="O6" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="6"/>
+      <c r="S6" s="1"/>
+      <c r="U6" s="1"/>
+      <c r="V6" s="6"/>
+      <c r="W6" s="82"/>
+      <c r="X6" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="Y6" s="1"/>
+      <c r="Z6" s="1"/>
+      <c r="AA6" s="6"/>
+      <c r="AB6" s="1"/>
+      <c r="AC6" s="1"/>
+    </row>
+    <row r="7" spans="2:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C7" s="1"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="82"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="82"/>
+      <c r="O7" s="11"/>
+      <c r="P7" s="5"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="6"/>
+      <c r="S7" s="1"/>
+      <c r="U7" s="1"/>
+      <c r="V7" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="W7" s="82"/>
+      <c r="X7" s="11"/>
+      <c r="Y7" s="5"/>
+      <c r="Z7" s="1"/>
+      <c r="AA7" s="6"/>
+      <c r="AB7" s="1"/>
+      <c r="AC7" s="1"/>
+    </row>
+    <row r="8" spans="2:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C8" s="1"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+      <c r="U8" s="1"/>
+      <c r="V8" s="7"/>
+      <c r="W8" s="1"/>
+      <c r="X8" s="1"/>
+      <c r="Y8" s="5"/>
+      <c r="Z8" s="1"/>
+      <c r="AA8" s="1"/>
+      <c r="AB8" s="1"/>
+      <c r="AC8" s="1"/>
+    </row>
+    <row r="9" spans="2:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C9" s="1"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6">
+        <v>8</v>
+      </c>
+      <c r="F9" s="6"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="O9" s="6"/>
+      <c r="P9" s="4"/>
+      <c r="Q9" s="5"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
+      <c r="U9" s="1"/>
+      <c r="V9" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="W9" s="4"/>
+      <c r="X9" s="5"/>
+      <c r="Y9" s="4"/>
+      <c r="Z9" s="5"/>
+      <c r="AA9" s="1"/>
+      <c r="AB9" s="1"/>
+      <c r="AC9" s="1"/>
+    </row>
+    <row r="10" spans="2:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C10" s="1"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="5"/>
+      <c r="Q10" s="5"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
+      <c r="U10" s="1"/>
+      <c r="V10" s="6"/>
+      <c r="W10" s="6"/>
+      <c r="X10" s="5"/>
+      <c r="Y10" s="5"/>
+      <c r="Z10" s="5"/>
+      <c r="AA10" s="1"/>
+      <c r="AB10" s="1"/>
+      <c r="AC10" s="1"/>
+    </row>
+    <row r="11" spans="2:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C11" s="1"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="8">
+        <v>9</v>
+      </c>
+      <c r="F11" s="20"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="O11" s="20"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="5"/>
+      <c r="R11" s="1"/>
+      <c r="S11" s="1"/>
+      <c r="U11" s="1"/>
+      <c r="V11" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="W11" s="6"/>
+      <c r="X11" s="4"/>
+      <c r="Y11" s="1"/>
+      <c r="Z11" s="5"/>
+      <c r="AA11" s="1"/>
+      <c r="AB11" s="1"/>
+      <c r="AC11" s="1"/>
+    </row>
+    <row r="12" spans="2:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C12" s="1"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="6"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="5"/>
+      <c r="R12" s="1"/>
+      <c r="S12" s="1"/>
+      <c r="U12" s="1"/>
+      <c r="V12" s="7"/>
+      <c r="W12" s="1"/>
+      <c r="X12" s="5"/>
+      <c r="Y12" s="1"/>
+      <c r="Z12" s="4"/>
+      <c r="AA12" s="5"/>
+      <c r="AB12" s="1"/>
+      <c r="AC12" s="1"/>
+    </row>
+    <row r="13" spans="2:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C13" s="1"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6">
+        <v>4</v>
+      </c>
+      <c r="F13" s="6"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="6"/>
+      <c r="N13" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="O13" s="6"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="4"/>
+      <c r="R13" s="5"/>
+      <c r="S13" s="1"/>
+      <c r="U13" s="1"/>
+      <c r="V13" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="W13" s="4"/>
+      <c r="X13" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="Y13" s="6"/>
+      <c r="Z13" s="5"/>
+      <c r="AA13" s="5"/>
+      <c r="AB13" s="1"/>
+      <c r="AC13" s="1"/>
+    </row>
+    <row r="14" spans="2:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C14" s="1"/>
+      <c r="D14" s="6">
+        <v>13</v>
+      </c>
+      <c r="E14" s="7"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="N14" s="7"/>
+      <c r="O14" s="6"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="5"/>
+      <c r="R14" s="5"/>
+      <c r="S14" s="1"/>
+      <c r="U14" s="1"/>
+      <c r="V14" s="1"/>
+      <c r="W14" s="1"/>
+      <c r="X14" s="7"/>
+      <c r="Y14" s="1"/>
+      <c r="Z14" s="5"/>
+      <c r="AA14" s="5"/>
+      <c r="AB14" s="1"/>
+      <c r="AC14" s="1"/>
+    </row>
+    <row r="15" spans="2:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C15" s="1"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="7"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="20"/>
+      <c r="P15" s="5"/>
+      <c r="Q15" s="5"/>
+      <c r="R15" s="5"/>
+      <c r="S15" s="1"/>
+      <c r="U15" s="1"/>
+      <c r="V15" s="1"/>
+      <c r="W15" s="1"/>
+      <c r="X15" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="Y15" s="4"/>
+      <c r="Z15" s="1"/>
+      <c r="AA15" s="5"/>
+      <c r="AB15" s="1"/>
+      <c r="AC15" s="1"/>
+    </row>
+    <row r="16" spans="2:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C16" s="1"/>
+      <c r="D16" s="8">
+        <v>14</v>
+      </c>
+      <c r="E16" s="4"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="N16" s="4"/>
+      <c r="O16" s="6"/>
+      <c r="P16" s="5"/>
+      <c r="Q16" s="5"/>
+      <c r="R16" s="5"/>
+      <c r="S16" s="1"/>
+      <c r="U16" s="1"/>
+      <c r="V16" s="1"/>
+      <c r="W16" s="1"/>
+      <c r="X16" s="1"/>
+      <c r="Y16" s="1"/>
+      <c r="Z16" s="1"/>
+      <c r="AA16" s="5"/>
+      <c r="AB16" s="1"/>
+      <c r="AC16" s="1"/>
+    </row>
+    <row r="17" spans="3:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C17" s="1"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6">
+        <v>5</v>
+      </c>
+      <c r="F17" s="6"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="6"/>
+      <c r="N17" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="O17" s="6"/>
+      <c r="P17" s="4"/>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="5"/>
+      <c r="S17" s="1"/>
+      <c r="U17" s="1"/>
+      <c r="V17" s="1"/>
+      <c r="W17" s="1"/>
+      <c r="X17" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="Y17" s="1"/>
+      <c r="Z17" s="1"/>
+      <c r="AA17" s="15"/>
+      <c r="AB17" s="1"/>
+      <c r="AC17" s="1"/>
+    </row>
+    <row r="18" spans="3:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C18" s="1"/>
+      <c r="D18" s="6">
+        <v>12</v>
+      </c>
+      <c r="E18" s="7"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="N18" s="7"/>
+      <c r="O18" s="6"/>
+      <c r="P18" s="5"/>
+      <c r="Q18" s="1"/>
+      <c r="R18" s="5"/>
+      <c r="S18" s="1"/>
+      <c r="U18" s="1"/>
+      <c r="V18" s="1"/>
+      <c r="W18" s="1"/>
+      <c r="X18" s="7"/>
+      <c r="Y18" s="1"/>
+      <c r="Z18" s="1"/>
+      <c r="AA18" s="84"/>
+      <c r="AB18" s="1"/>
+      <c r="AC18" s="1"/>
+    </row>
+    <row r="19" spans="3:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C19" s="1"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="7"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="20"/>
+      <c r="P19" s="1"/>
+      <c r="Q19" s="1"/>
+      <c r="R19" s="5"/>
+      <c r="S19" s="1"/>
+      <c r="U19" s="1"/>
+      <c r="V19" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="W19" s="1"/>
+      <c r="X19" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="Y19" s="4"/>
+      <c r="Z19" s="5"/>
+      <c r="AA19" s="84"/>
+      <c r="AB19" s="1"/>
+      <c r="AC19" s="1"/>
+    </row>
+    <row r="20" spans="3:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C20" s="1"/>
+      <c r="D20" s="8">
+        <v>15</v>
+      </c>
+      <c r="E20" s="4"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="N20" s="4"/>
+      <c r="O20" s="6"/>
+      <c r="P20" s="6"/>
+      <c r="Q20" s="1"/>
+      <c r="R20" s="5"/>
+      <c r="S20" s="1"/>
+      <c r="U20" s="1"/>
+      <c r="V20" s="7"/>
+      <c r="W20" s="1"/>
+      <c r="X20" s="1"/>
+      <c r="Y20" s="1"/>
+      <c r="Z20" s="5"/>
+      <c r="AA20" s="84"/>
+      <c r="AB20" s="1"/>
+      <c r="AC20" s="1"/>
+    </row>
+    <row r="21" spans="3:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C21" s="1"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="6"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="6"/>
+      <c r="P21" s="1"/>
+      <c r="Q21" s="1"/>
+      <c r="R21" s="4"/>
+      <c r="S21" s="1"/>
+      <c r="U21" s="82"/>
+      <c r="V21" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="W21" s="4"/>
+      <c r="X21" s="5"/>
+      <c r="Y21" s="1"/>
+      <c r="Z21" s="5"/>
+      <c r="AA21" s="84"/>
+      <c r="AB21" s="1"/>
+      <c r="AC21" s="1"/>
+    </row>
+    <row r="22" spans="3:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C22" s="1"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="82"/>
+      <c r="F22" s="6">
+        <v>3</v>
+      </c>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="6"/>
+      <c r="N22" s="82"/>
+      <c r="O22" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="P22" s="1"/>
+      <c r="Q22" s="1"/>
+      <c r="R22" s="5"/>
+      <c r="S22" s="1"/>
+      <c r="U22" s="82"/>
+      <c r="V22" s="6"/>
+      <c r="W22" s="6"/>
+      <c r="X22" s="5"/>
+      <c r="Y22" s="1"/>
+      <c r="Z22" s="4"/>
+      <c r="AA22" s="14"/>
+      <c r="AB22" s="4"/>
+      <c r="AC22" s="1"/>
+    </row>
+    <row r="23" spans="3:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C23" s="1"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="82"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="6"/>
+      <c r="N23" s="82"/>
+      <c r="O23" s="11"/>
+      <c r="P23" s="5"/>
+      <c r="Q23" s="1"/>
+      <c r="R23" s="5"/>
+      <c r="S23" s="1"/>
+      <c r="U23" s="82"/>
+      <c r="V23" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="W23" s="6"/>
+      <c r="X23" s="4"/>
+      <c r="Y23" s="5"/>
+      <c r="Z23" s="5"/>
+      <c r="AA23" s="14"/>
+      <c r="AB23" s="1"/>
+      <c r="AC23" s="1"/>
+    </row>
+    <row r="24" spans="3:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C24" s="1"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="1"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="6"/>
+      <c r="N24" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="O24" s="6"/>
+      <c r="P24" s="5"/>
+      <c r="Q24" s="1"/>
+      <c r="R24" s="5"/>
+      <c r="S24" s="1"/>
+      <c r="U24" s="82"/>
+      <c r="V24" s="7"/>
+      <c r="W24" s="1"/>
+      <c r="X24" s="5"/>
+      <c r="Y24" s="5"/>
+      <c r="Z24" s="5"/>
+      <c r="AA24" s="14"/>
+      <c r="AB24" s="1"/>
+      <c r="AC24" s="1"/>
+    </row>
+    <row r="25" spans="3:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C25" s="1"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6">
+        <v>6</v>
+      </c>
+      <c r="F25" s="6"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="1"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="6"/>
+      <c r="N25" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="O25" s="6"/>
+      <c r="P25" s="4"/>
+      <c r="Q25" s="5"/>
+      <c r="R25" s="5"/>
+      <c r="S25" s="1"/>
+      <c r="U25" s="82"/>
+      <c r="V25" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="W25" s="4"/>
+      <c r="X25" s="6"/>
+      <c r="Y25" s="4"/>
+      <c r="Z25" s="82"/>
+      <c r="AA25" s="14"/>
+      <c r="AB25" s="1"/>
+      <c r="AC25" s="1"/>
+    </row>
+    <row r="26" spans="3:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C26" s="1"/>
+      <c r="D26" s="6">
+        <v>11</v>
+      </c>
+      <c r="E26" s="7"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="5"/>
+      <c r="J26" s="1"/>
+      <c r="L26" s="1"/>
+      <c r="M26" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="N26" s="7"/>
+      <c r="O26" s="6"/>
+      <c r="P26" s="5"/>
+      <c r="Q26" s="5"/>
+      <c r="R26" s="5"/>
+      <c r="S26" s="1"/>
+      <c r="U26" s="82"/>
+      <c r="V26" s="83"/>
+      <c r="W26" s="83"/>
+      <c r="X26" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="Y26" s="5"/>
+      <c r="Z26" s="82"/>
+      <c r="AA26" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="AB26" s="1"/>
+      <c r="AC26" s="1"/>
+    </row>
+    <row r="27" spans="3:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C27" s="1"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="5"/>
+      <c r="J27" s="1"/>
+      <c r="L27" s="1"/>
+      <c r="M27" s="7"/>
+      <c r="N27" s="1"/>
+      <c r="O27" s="20"/>
+      <c r="P27" s="1"/>
+      <c r="Q27" s="5"/>
+      <c r="R27" s="5"/>
+      <c r="S27" s="1"/>
+      <c r="U27" s="82"/>
+      <c r="V27" s="83"/>
+      <c r="W27" s="82"/>
+      <c r="X27" s="83"/>
+      <c r="Y27" s="82"/>
+      <c r="Z27" s="82"/>
+      <c r="AA27" s="82"/>
+      <c r="AB27" s="1"/>
+      <c r="AC27" s="1"/>
+    </row>
+    <row r="28" spans="3:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C28" s="1"/>
+      <c r="D28" s="8">
+        <v>16</v>
+      </c>
+      <c r="E28" s="4"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="5"/>
+      <c r="J28" s="1"/>
+      <c r="L28" s="1"/>
+      <c r="M28" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="N28" s="4"/>
+      <c r="O28" s="6"/>
+      <c r="P28" s="1"/>
+      <c r="Q28" s="5"/>
+      <c r="R28" s="5"/>
+      <c r="S28" s="1"/>
+      <c r="U28" s="82"/>
+      <c r="V28" s="83"/>
+      <c r="W28" s="82"/>
+      <c r="X28" s="83"/>
+      <c r="Y28" s="82"/>
+      <c r="Z28" s="82"/>
+      <c r="AA28" s="82"/>
+      <c r="AB28" s="1"/>
+      <c r="AC28" s="1"/>
+    </row>
+    <row r="29" spans="3:29" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="C29" s="1"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+      <c r="L29" s="1"/>
+      <c r="M29" s="6"/>
+      <c r="N29" s="1"/>
+      <c r="O29" s="6"/>
+      <c r="P29" s="1"/>
+      <c r="Q29" s="4"/>
+      <c r="R29" s="1"/>
+      <c r="S29" s="1"/>
+      <c r="U29" s="82"/>
+      <c r="V29" s="83"/>
+      <c r="W29" s="82"/>
+      <c r="X29" s="83"/>
+      <c r="Y29" s="82"/>
+      <c r="Z29" s="82"/>
+      <c r="AA29" s="1"/>
+      <c r="AB29" s="1"/>
+      <c r="AC29" s="1"/>
+    </row>
+    <row r="30" spans="3:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C30" s="1"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="82"/>
+      <c r="F30" s="6">
         <v>2</v>
       </c>
-      <c r="E4">
-        <v>3</v>
-      </c>
-      <c r="F4">
-        <v>4</v>
-      </c>
-      <c r="G4">
-        <v>5</v>
-      </c>
-      <c r="H4">
-        <v>6</v>
-      </c>
-      <c r="I4">
+      <c r="G30" s="1"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+      <c r="L30" s="1"/>
+      <c r="M30" s="6"/>
+      <c r="N30" s="82"/>
+      <c r="O30" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="P30" s="1"/>
+      <c r="Q30" s="5"/>
+      <c r="R30" s="1"/>
+      <c r="S30" s="1"/>
+      <c r="U30" s="82"/>
+      <c r="V30" s="83"/>
+      <c r="W30" s="82"/>
+      <c r="X30" s="83"/>
+      <c r="Y30" s="82"/>
+      <c r="Z30" s="82"/>
+      <c r="AA30" s="1"/>
+      <c r="AB30" s="1"/>
+      <c r="AC30" s="1"/>
+    </row>
+    <row r="31" spans="3:29" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="C31" s="1"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="82"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
+      <c r="L31" s="1"/>
+      <c r="M31" s="6"/>
+      <c r="N31" s="82"/>
+      <c r="O31" s="11"/>
+      <c r="P31" s="5"/>
+      <c r="Q31" s="5"/>
+      <c r="R31" s="1"/>
+      <c r="S31" s="1"/>
+      <c r="U31" s="82"/>
+      <c r="V31" s="83"/>
+      <c r="W31" s="82"/>
+      <c r="X31" s="83"/>
+      <c r="Y31" s="82"/>
+      <c r="Z31" s="82"/>
+      <c r="AA31" s="1"/>
+      <c r="AB31" s="1"/>
+      <c r="AC31" s="1"/>
+    </row>
+    <row r="32" spans="3:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C32" s="1"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
+      <c r="L32" s="1"/>
+      <c r="M32" s="6"/>
+      <c r="N32" s="6"/>
+      <c r="O32" s="6"/>
+      <c r="P32" s="5"/>
+      <c r="Q32" s="5"/>
+      <c r="R32" s="1"/>
+      <c r="S32" s="1"/>
+      <c r="U32" s="82"/>
+      <c r="V32" s="83"/>
+      <c r="W32" s="83"/>
+      <c r="X32" s="83"/>
+      <c r="Y32" s="82"/>
+      <c r="Z32" s="82"/>
+      <c r="AA32" s="1"/>
+      <c r="AB32" s="1"/>
+      <c r="AC32" s="1"/>
+    </row>
+    <row r="33" spans="3:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C33" s="1"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6">
         <v>7</v>
       </c>
-      <c r="J4">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5">
-        <v>2</v>
-      </c>
-      <c r="E5">
-        <v>3</v>
-      </c>
-      <c r="F5">
-        <v>4</v>
-      </c>
-      <c r="G5">
-        <v>5</v>
-      </c>
-      <c r="H5">
-        <v>7</v>
-      </c>
-      <c r="I5">
-        <v>6</v>
-      </c>
-      <c r="J5">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6">
-        <v>2</v>
-      </c>
-      <c r="E6">
-        <v>3</v>
-      </c>
-      <c r="F6">
-        <v>4</v>
-      </c>
-      <c r="G6">
-        <v>5</v>
-      </c>
-      <c r="H6">
-        <v>8</v>
-      </c>
-      <c r="I6">
-        <v>6</v>
-      </c>
-      <c r="J6">
-        <v>7</v>
-      </c>
+      <c r="F33" s="6"/>
+      <c r="G33" s="4"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+      <c r="L33" s="1"/>
+      <c r="M33" s="6"/>
+      <c r="N33" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="O33" s="6"/>
+      <c r="P33" s="4"/>
+      <c r="Q33" s="1"/>
+      <c r="R33" s="1"/>
+      <c r="S33" s="1"/>
+      <c r="U33" s="82"/>
+      <c r="V33" s="83"/>
+      <c r="W33" s="83"/>
+      <c r="X33" s="83"/>
+      <c r="Y33" s="82"/>
+      <c r="Z33" s="82"/>
+      <c r="AA33" s="1"/>
+      <c r="AB33" s="1"/>
+      <c r="AC33" s="1"/>
+    </row>
+    <row r="34" spans="3:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C34" s="1"/>
+      <c r="D34" s="6">
+        <v>10</v>
+      </c>
+      <c r="E34" s="7"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="5"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+      <c r="J34" s="1"/>
+      <c r="L34" s="1"/>
+      <c r="M34" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="N34" s="7"/>
+      <c r="O34" s="6"/>
+      <c r="P34" s="5"/>
+      <c r="Q34" s="1"/>
+      <c r="R34" s="1"/>
+      <c r="S34" s="1"/>
+      <c r="U34" s="82"/>
+      <c r="V34" s="83"/>
+      <c r="W34" s="83"/>
+      <c r="X34" s="83"/>
+      <c r="Y34" s="82"/>
+      <c r="Z34" s="82"/>
+      <c r="AA34" s="1"/>
+      <c r="AB34" s="1"/>
+      <c r="AC34" s="1"/>
+    </row>
+    <row r="35" spans="3:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C35" s="1"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="20"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
+      <c r="J35" s="1"/>
+      <c r="L35" s="1"/>
+      <c r="M35" s="7"/>
+      <c r="N35" s="1"/>
+      <c r="O35" s="20"/>
+      <c r="P35" s="1"/>
+      <c r="Q35" s="1"/>
+      <c r="R35" s="1"/>
+      <c r="S35" s="1"/>
+      <c r="U35" s="82"/>
+      <c r="V35" s="83"/>
+      <c r="W35" s="82"/>
+      <c r="X35" s="83"/>
+      <c r="Y35" s="82"/>
+      <c r="Z35" s="82"/>
+      <c r="AA35" s="1"/>
+      <c r="AB35" s="1"/>
+      <c r="AC35" s="1"/>
+    </row>
+    <row r="36" spans="3:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C36" s="1"/>
+      <c r="D36" s="8">
+        <v>17</v>
+      </c>
+      <c r="E36" s="4"/>
+      <c r="F36" s="6"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+      <c r="J36" s="1"/>
+      <c r="L36" s="1"/>
+      <c r="M36" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="N36" s="4"/>
+      <c r="O36" s="6"/>
+      <c r="P36" s="1"/>
+      <c r="Q36" s="1"/>
+      <c r="R36" s="1"/>
+      <c r="S36" s="1"/>
+      <c r="U36" s="82"/>
+      <c r="V36" s="83"/>
+      <c r="W36" s="82"/>
+      <c r="X36" s="83"/>
+      <c r="Y36" s="82"/>
+      <c r="Z36" s="82"/>
+      <c r="AA36" s="1"/>
+      <c r="AB36" s="1"/>
+      <c r="AC36" s="1"/>
+    </row>
+    <row r="37" spans="3:29" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="C37" s="1"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="6"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+      <c r="J37" s="1"/>
+      <c r="L37" s="1"/>
+      <c r="M37" s="6"/>
+      <c r="N37" s="1"/>
+      <c r="O37" s="6"/>
+      <c r="P37" s="1"/>
+      <c r="Q37" s="1"/>
+      <c r="R37" s="1"/>
+      <c r="S37" s="1"/>
+      <c r="U37" s="82"/>
+      <c r="V37" s="83"/>
+      <c r="W37" s="82"/>
+      <c r="X37" s="83"/>
+      <c r="Y37" s="82"/>
+      <c r="Z37" s="82"/>
+      <c r="AA37" s="1"/>
+      <c r="AB37" s="1"/>
+      <c r="AC37" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4934,8 +5945,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D84D55B-86DB-41A7-86B6-8D3E6C4FEE99}">
   <dimension ref="C4:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L27" sqref="L27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9455,32 +10466,32 @@
       <c r="I9" s="5"/>
     </row>
     <row r="10" spans="2:9" ht="4.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="75" t="s">
+      <c r="B10" s="76" t="s">
         <v>25</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="79"/>
-      <c r="F10" s="74"/>
+      <c r="E10" s="78"/>
+      <c r="F10" s="79"/>
       <c r="G10" s="6"/>
       <c r="H10" s="1"/>
       <c r="I10" s="5"/>
     </row>
     <row r="11" spans="2:9" ht="4.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="75"/>
+      <c r="B11" s="76"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="79"/>
-      <c r="F11" s="74"/>
+      <c r="E11" s="78"/>
+      <c r="F11" s="79"/>
       <c r="G11" s="6"/>
       <c r="H11" s="1"/>
       <c r="I11" s="5"/>
     </row>
     <row r="12" spans="2:9" ht="4.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="76"/>
+      <c r="B12" s="77"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="74"/>
+      <c r="E12" s="79"/>
       <c r="F12" s="1"/>
       <c r="G12" s="6"/>
       <c r="H12" s="1"/>
@@ -9488,37 +10499,37 @@
     </row>
     <row r="13" spans="2:9" ht="4.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B13" s="2"/>
-      <c r="C13" s="75" t="s">
+      <c r="C13" s="76" t="s">
         <v>29</v>
       </c>
       <c r="D13" s="1"/>
-      <c r="E13" s="74"/>
+      <c r="E13" s="79"/>
       <c r="F13" s="1"/>
       <c r="G13" s="6"/>
       <c r="H13" s="1"/>
-      <c r="I13" s="77" t="s">
+      <c r="I13" s="74" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="14" spans="2:9" ht="4.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="14"/>
-      <c r="C14" s="75"/>
-      <c r="D14" s="74"/>
-      <c r="E14" s="79"/>
+      <c r="C14" s="76"/>
+      <c r="D14" s="79"/>
+      <c r="E14" s="78"/>
       <c r="F14" s="1"/>
       <c r="G14" s="6"/>
       <c r="H14" s="1"/>
-      <c r="I14" s="77"/>
+      <c r="I14" s="74"/>
     </row>
     <row r="15" spans="2:9" ht="4.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="18"/>
-      <c r="C15" s="76"/>
-      <c r="D15" s="74"/>
-      <c r="E15" s="79"/>
+      <c r="C15" s="77"/>
+      <c r="D15" s="79"/>
+      <c r="E15" s="78"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
-      <c r="I15" s="78"/>
+      <c r="I15" s="75"/>
     </row>
     <row r="16" spans="2:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="8" t="s">
@@ -9606,17 +10617,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="I13:I15"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="E14:E15"/>
     <mergeCell ref="D20:F21"/>
     <mergeCell ref="F16:F17"/>
     <mergeCell ref="F10:F11"/>
     <mergeCell ref="C13:C15"/>
     <mergeCell ref="D14:D15"/>
     <mergeCell ref="E12:E13"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="I13:I15"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="E14:E15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fleshed out Simple Mulitbrackets and developed notes.txt
</commit_message>
<xml_diff>
--- a/thesis-tex/images/Brackets/Brackets.xlsx
+++ b/thesis-tex/images/Brackets/Brackets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leofr\Documents\LeoWork\School\04College\17Senior\thesis\thesis-tex\images\Brackets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62D599C9-4C05-4B6F-82C8-3D7C5D2A9B51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80185915-6F29-49BF-8F58-2B640A94ACEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="9" activeTab="17" xr2:uid="{503DA620-194E-433E-B5EB-5393E7537419}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="9" activeTab="15" xr2:uid="{503DA620-194E-433E-B5EB-5393E7537419}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="116">
   <si>
     <t>Georgia</t>
   </si>
@@ -399,6 +399,9 @@
   </si>
   <si>
     <t>Tier 6</t>
+  </si>
+  <si>
+    <t>G1</t>
   </si>
 </sst>
 </file>
@@ -979,8 +982,18 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -989,15 +1002,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1006,11 +1010,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3321,10 +3326,10 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BF5E35F-6BAF-409B-A5CF-ACCF63F9A711}">
-  <dimension ref="B4:AI28"/>
+  <dimension ref="B4:AX28"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="Y25" sqref="Y25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3335,7 +3340,7 @@
     <col min="9" max="10" width="10.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:50" x14ac:dyDescent="0.3">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -3370,8 +3375,23 @@
       <c r="AG4" s="1"/>
       <c r="AH4" s="1"/>
       <c r="AI4" s="1"/>
-    </row>
-    <row r="5" spans="2:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AJ4" s="1"/>
+      <c r="AK4" s="1"/>
+      <c r="AL4" s="1"/>
+      <c r="AM4" s="1"/>
+      <c r="AN4" s="1"/>
+      <c r="AO4" s="1"/>
+      <c r="AP4" s="1"/>
+      <c r="AQ4" s="1"/>
+      <c r="AR4" s="1"/>
+      <c r="AS4" s="1"/>
+      <c r="AT4" s="1"/>
+      <c r="AU4" s="1"/>
+      <c r="AV4" s="1"/>
+      <c r="AW4" s="1"/>
+      <c r="AX4" s="1"/>
+    </row>
+    <row r="5" spans="2:50" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="1"/>
       <c r="C5" s="6">
         <v>1</v>
@@ -3418,8 +3438,27 @@
       <c r="AG5" s="1"/>
       <c r="AH5" s="1"/>
       <c r="AI5" s="1"/>
-    </row>
-    <row r="6" spans="2:35" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AJ5" s="6">
+        <v>1</v>
+      </c>
+      <c r="AK5" s="1"/>
+      <c r="AL5" s="1"/>
+      <c r="AM5" s="1"/>
+      <c r="AN5" s="1"/>
+      <c r="AO5" s="1"/>
+      <c r="AP5" s="6">
+        <v>1</v>
+      </c>
+      <c r="AQ5" s="1"/>
+      <c r="AR5" s="1"/>
+      <c r="AS5" s="1"/>
+      <c r="AT5" s="1"/>
+      <c r="AU5" s="1"/>
+      <c r="AV5" s="1"/>
+      <c r="AW5" s="1"/>
+      <c r="AX5" s="1"/>
+    </row>
+    <row r="6" spans="2:50" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="1"/>
       <c r="C6" s="66" t="s">
         <v>59</v>
@@ -3466,8 +3505,27 @@
       <c r="AG6" s="1"/>
       <c r="AH6" s="1"/>
       <c r="AI6" s="1"/>
-    </row>
-    <row r="7" spans="2:35" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AJ6" s="66" t="s">
+        <v>59</v>
+      </c>
+      <c r="AK6" s="1"/>
+      <c r="AL6" s="1"/>
+      <c r="AM6" s="1"/>
+      <c r="AN6" s="1"/>
+      <c r="AO6" s="1"/>
+      <c r="AP6" s="66" t="s">
+        <v>59</v>
+      </c>
+      <c r="AQ6" s="1"/>
+      <c r="AR6" s="1"/>
+      <c r="AS6" s="1"/>
+      <c r="AT6" s="1"/>
+      <c r="AU6" s="1"/>
+      <c r="AV6" s="1"/>
+      <c r="AW6" s="1"/>
+      <c r="AX6" s="1"/>
+    </row>
+    <row r="7" spans="2:50" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="1"/>
       <c r="C7" s="8">
         <v>8</v>
@@ -3514,8 +3572,27 @@
       <c r="AG7" s="1"/>
       <c r="AH7" s="1"/>
       <c r="AI7" s="1"/>
-    </row>
-    <row r="8" spans="2:35" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AJ7" s="8">
+        <v>8</v>
+      </c>
+      <c r="AK7" s="4"/>
+      <c r="AL7" s="5"/>
+      <c r="AM7" s="1"/>
+      <c r="AN7" s="1"/>
+      <c r="AO7" s="1"/>
+      <c r="AP7" s="8">
+        <v>8</v>
+      </c>
+      <c r="AQ7" s="4"/>
+      <c r="AR7" s="5"/>
+      <c r="AS7" s="1"/>
+      <c r="AT7" s="1"/>
+      <c r="AU7" s="1"/>
+      <c r="AV7" s="1"/>
+      <c r="AW7" s="1"/>
+      <c r="AX7" s="1"/>
+    </row>
+    <row r="8" spans="2:50" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="1"/>
       <c r="C8" s="6"/>
       <c r="D8" s="59" t="s">
@@ -3562,8 +3639,27 @@
       <c r="AG8" s="1"/>
       <c r="AH8" s="1"/>
       <c r="AI8" s="1"/>
-    </row>
-    <row r="9" spans="2:35" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AJ8" s="6"/>
+      <c r="AK8" s="59" t="s">
+        <v>63</v>
+      </c>
+      <c r="AL8" s="5"/>
+      <c r="AM8" s="1"/>
+      <c r="AN8" s="1"/>
+      <c r="AO8" s="1"/>
+      <c r="AP8" s="6"/>
+      <c r="AQ8" s="59" t="s">
+        <v>63</v>
+      </c>
+      <c r="AR8" s="5"/>
+      <c r="AS8" s="1"/>
+      <c r="AT8" s="1"/>
+      <c r="AU8" s="1"/>
+      <c r="AV8" s="1"/>
+      <c r="AW8" s="1"/>
+      <c r="AX8" s="1"/>
+    </row>
+    <row r="9" spans="2:50" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="1"/>
       <c r="C9" s="6">
         <v>4</v>
@@ -3610,8 +3706,27 @@
       <c r="AG9" s="5"/>
       <c r="AH9" s="1"/>
       <c r="AI9" s="1"/>
-    </row>
-    <row r="10" spans="2:35" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AJ9" s="6">
+        <v>4</v>
+      </c>
+      <c r="AK9" s="1"/>
+      <c r="AL9" s="4"/>
+      <c r="AM9" s="5"/>
+      <c r="AN9" s="1"/>
+      <c r="AO9" s="1"/>
+      <c r="AP9" s="6">
+        <v>4</v>
+      </c>
+      <c r="AQ9" s="1"/>
+      <c r="AR9" s="4"/>
+      <c r="AS9" s="5"/>
+      <c r="AT9" s="1"/>
+      <c r="AU9" s="1"/>
+      <c r="AV9" s="1"/>
+      <c r="AW9" s="1"/>
+      <c r="AX9" s="1"/>
+    </row>
+    <row r="10" spans="2:50" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="1"/>
       <c r="C10" s="66" t="s">
         <v>60</v>
@@ -3658,8 +3773,27 @@
       <c r="AG10" s="5"/>
       <c r="AH10" s="1"/>
       <c r="AI10" s="1"/>
-    </row>
-    <row r="11" spans="2:35" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AJ10" s="66" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK10" s="1"/>
+      <c r="AL10" s="5"/>
+      <c r="AM10" s="5"/>
+      <c r="AN10" s="1"/>
+      <c r="AO10" s="1"/>
+      <c r="AP10" s="66" t="s">
+        <v>60</v>
+      </c>
+      <c r="AQ10" s="1"/>
+      <c r="AR10" s="5"/>
+      <c r="AS10" s="5"/>
+      <c r="AT10" s="1"/>
+      <c r="AU10" s="1"/>
+      <c r="AV10" s="1"/>
+      <c r="AW10" s="1"/>
+      <c r="AX10" s="1"/>
+    </row>
+    <row r="11" spans="2:50" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="1"/>
       <c r="C11" s="8">
         <v>5</v>
@@ -3706,8 +3840,27 @@
       <c r="AG11" s="5"/>
       <c r="AH11" s="1"/>
       <c r="AI11" s="1"/>
-    </row>
-    <row r="12" spans="2:35" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AJ11" s="8">
+        <v>5</v>
+      </c>
+      <c r="AK11" s="4"/>
+      <c r="AL11" s="1"/>
+      <c r="AM11" s="5"/>
+      <c r="AN11" s="1"/>
+      <c r="AO11" s="1"/>
+      <c r="AP11" s="8">
+        <v>5</v>
+      </c>
+      <c r="AQ11" s="4"/>
+      <c r="AR11" s="1"/>
+      <c r="AS11" s="5"/>
+      <c r="AT11" s="1"/>
+      <c r="AU11" s="1"/>
+      <c r="AV11" s="1"/>
+      <c r="AW11" s="1"/>
+      <c r="AX11" s="1"/>
+    </row>
+    <row r="12" spans="2:50" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="1"/>
       <c r="C12" s="6"/>
       <c r="D12" s="1"/>
@@ -3754,8 +3907,27 @@
       <c r="AG12" s="5"/>
       <c r="AH12" s="1"/>
       <c r="AI12" s="1"/>
-    </row>
-    <row r="13" spans="2:35" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AJ12" s="6"/>
+      <c r="AK12" s="1"/>
+      <c r="AL12" s="59" t="s">
+        <v>65</v>
+      </c>
+      <c r="AM12" s="5"/>
+      <c r="AN12" s="1"/>
+      <c r="AO12" s="1"/>
+      <c r="AP12" s="6"/>
+      <c r="AQ12" s="1"/>
+      <c r="AR12" s="59" t="s">
+        <v>65</v>
+      </c>
+      <c r="AS12" s="5"/>
+      <c r="AT12" s="1"/>
+      <c r="AU12" s="1"/>
+      <c r="AV12" s="1"/>
+      <c r="AW12" s="1"/>
+      <c r="AX12" s="1"/>
+    </row>
+    <row r="13" spans="2:50" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="1"/>
       <c r="C13" s="6">
         <v>3</v>
@@ -3802,8 +3974,27 @@
       <c r="AG13" s="4"/>
       <c r="AH13" s="1"/>
       <c r="AI13" s="1"/>
-    </row>
-    <row r="14" spans="2:35" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AJ13" s="6">
+        <v>3</v>
+      </c>
+      <c r="AK13" s="1"/>
+      <c r="AL13" s="1"/>
+      <c r="AM13" s="4"/>
+      <c r="AN13" s="1"/>
+      <c r="AO13" s="1"/>
+      <c r="AP13" s="6">
+        <v>3</v>
+      </c>
+      <c r="AQ13" s="1"/>
+      <c r="AR13" s="1"/>
+      <c r="AS13" s="4"/>
+      <c r="AT13" s="1"/>
+      <c r="AU13" s="1"/>
+      <c r="AV13" s="1"/>
+      <c r="AW13" s="1"/>
+      <c r="AX13" s="1"/>
+    </row>
+    <row r="14" spans="2:50" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="1"/>
       <c r="C14" s="66" t="s">
         <v>61</v>
@@ -3850,8 +4041,27 @@
       <c r="AG14" s="5"/>
       <c r="AH14" s="1"/>
       <c r="AI14" s="1"/>
-    </row>
-    <row r="15" spans="2:35" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AJ14" s="66" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK14" s="1"/>
+      <c r="AL14" s="1"/>
+      <c r="AM14" s="5"/>
+      <c r="AN14" s="1"/>
+      <c r="AO14" s="1"/>
+      <c r="AP14" s="66" t="s">
+        <v>61</v>
+      </c>
+      <c r="AQ14" s="1"/>
+      <c r="AR14" s="1"/>
+      <c r="AS14" s="5"/>
+      <c r="AT14" s="1"/>
+      <c r="AU14" s="1"/>
+      <c r="AV14" s="1"/>
+      <c r="AW14" s="1"/>
+      <c r="AX14" s="1"/>
+    </row>
+    <row r="15" spans="2:50" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="1"/>
       <c r="C15" s="8">
         <v>6</v>
@@ -3898,8 +4108,27 @@
       <c r="AG15" s="5"/>
       <c r="AH15" s="1"/>
       <c r="AI15" s="1"/>
-    </row>
-    <row r="16" spans="2:35" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AJ15" s="8">
+        <v>6</v>
+      </c>
+      <c r="AK15" s="4"/>
+      <c r="AL15" s="5"/>
+      <c r="AM15" s="5"/>
+      <c r="AN15" s="1"/>
+      <c r="AO15" s="1"/>
+      <c r="AP15" s="8">
+        <v>6</v>
+      </c>
+      <c r="AQ15" s="4"/>
+      <c r="AR15" s="5"/>
+      <c r="AS15" s="5"/>
+      <c r="AT15" s="1"/>
+      <c r="AU15" s="1"/>
+      <c r="AV15" s="1"/>
+      <c r="AW15" s="1"/>
+      <c r="AX15" s="1"/>
+    </row>
+    <row r="16" spans="2:50" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="1"/>
       <c r="C16" s="6"/>
       <c r="D16" s="59" t="s">
@@ -3946,8 +4175,27 @@
       <c r="AG16" s="5"/>
       <c r="AH16" s="1"/>
       <c r="AI16" s="1"/>
-    </row>
-    <row r="17" spans="2:35" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AJ16" s="6"/>
+      <c r="AK16" s="59" t="s">
+        <v>64</v>
+      </c>
+      <c r="AL16" s="5"/>
+      <c r="AM16" s="5"/>
+      <c r="AN16" s="1"/>
+      <c r="AO16" s="1"/>
+      <c r="AP16" s="6"/>
+      <c r="AQ16" s="59" t="s">
+        <v>64</v>
+      </c>
+      <c r="AR16" s="5"/>
+      <c r="AS16" s="5"/>
+      <c r="AT16" s="1"/>
+      <c r="AU16" s="1"/>
+      <c r="AV16" s="1"/>
+      <c r="AW16" s="1"/>
+      <c r="AX16" s="1"/>
+    </row>
+    <row r="17" spans="2:50" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="1"/>
       <c r="C17" s="6">
         <v>2</v>
@@ -3994,8 +4242,27 @@
       <c r="AG17" s="1"/>
       <c r="AH17" s="1"/>
       <c r="AI17" s="1"/>
-    </row>
-    <row r="18" spans="2:35" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AJ17" s="6">
+        <v>2</v>
+      </c>
+      <c r="AK17" s="1"/>
+      <c r="AL17" s="4"/>
+      <c r="AM17" s="1"/>
+      <c r="AN17" s="1"/>
+      <c r="AO17" s="1"/>
+      <c r="AP17" s="6">
+        <v>2</v>
+      </c>
+      <c r="AQ17" s="1"/>
+      <c r="AR17" s="4"/>
+      <c r="AS17" s="1"/>
+      <c r="AT17" s="1"/>
+      <c r="AU17" s="1"/>
+      <c r="AV17" s="1"/>
+      <c r="AW17" s="1"/>
+      <c r="AX17" s="1"/>
+    </row>
+    <row r="18" spans="2:50" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="1"/>
       <c r="C18" s="66" t="s">
         <v>62</v>
@@ -4046,8 +4313,27 @@
       <c r="AG18" s="1"/>
       <c r="AH18" s="1"/>
       <c r="AI18" s="1"/>
-    </row>
-    <row r="19" spans="2:35" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AJ18" s="66" t="s">
+        <v>62</v>
+      </c>
+      <c r="AK18" s="1"/>
+      <c r="AL18" s="5"/>
+      <c r="AM18" s="1"/>
+      <c r="AN18" s="1"/>
+      <c r="AO18" s="1"/>
+      <c r="AP18" s="66" t="s">
+        <v>62</v>
+      </c>
+      <c r="AQ18" s="1"/>
+      <c r="AR18" s="5"/>
+      <c r="AS18" s="1"/>
+      <c r="AT18" s="1"/>
+      <c r="AU18" s="1"/>
+      <c r="AV18" s="1"/>
+      <c r="AW18" s="1"/>
+      <c r="AX18" s="1"/>
+    </row>
+    <row r="19" spans="2:50" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="1"/>
       <c r="C19" s="8">
         <v>7</v>
@@ -4096,8 +4382,29 @@
       <c r="AG19" s="1"/>
       <c r="AH19" s="1"/>
       <c r="AI19" s="1"/>
-    </row>
-    <row r="20" spans="2:35" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AJ19" s="8">
+        <v>7</v>
+      </c>
+      <c r="AK19" s="4"/>
+      <c r="AL19" s="1"/>
+      <c r="AM19" s="1"/>
+      <c r="AN19" s="1"/>
+      <c r="AO19" s="1"/>
+      <c r="AP19" s="8">
+        <v>7</v>
+      </c>
+      <c r="AQ19" s="4"/>
+      <c r="AR19" s="1"/>
+      <c r="AS19" s="1"/>
+      <c r="AT19" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AU19" s="1"/>
+      <c r="AV19" s="1"/>
+      <c r="AW19" s="1"/>
+      <c r="AX19" s="1"/>
+    </row>
+    <row r="20" spans="2:50" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -4146,8 +4453,27 @@
       <c r="AG20" s="1"/>
       <c r="AH20" s="1"/>
       <c r="AI20" s="1"/>
-    </row>
-    <row r="21" spans="2:35" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AJ20" s="1"/>
+      <c r="AK20" s="1"/>
+      <c r="AL20" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="AM20" s="1"/>
+      <c r="AN20" s="1"/>
+      <c r="AO20" s="1"/>
+      <c r="AP20" s="1"/>
+      <c r="AQ20" s="1"/>
+      <c r="AR20" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="AS20" s="1"/>
+      <c r="AT20" s="66"/>
+      <c r="AU20" s="5"/>
+      <c r="AV20" s="1"/>
+      <c r="AW20" s="1"/>
+      <c r="AX20" s="1"/>
+    </row>
+    <row r="21" spans="2:50" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
@@ -4196,8 +4522,33 @@
       <c r="AG21" s="1"/>
       <c r="AH21" s="1"/>
       <c r="AI21" s="1"/>
-    </row>
-    <row r="22" spans="2:35" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AJ21" s="1"/>
+      <c r="AK21" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="AL21" s="66" t="s">
+        <v>81</v>
+      </c>
+      <c r="AM21" s="1"/>
+      <c r="AN21" s="1"/>
+      <c r="AO21" s="1"/>
+      <c r="AP21" s="1"/>
+      <c r="AQ21" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="AR21" s="66" t="s">
+        <v>81</v>
+      </c>
+      <c r="AS21" s="1"/>
+      <c r="AT21" s="59" t="s">
+        <v>115</v>
+      </c>
+      <c r="AU21" s="5"/>
+      <c r="AV21" s="1"/>
+      <c r="AW21" s="1"/>
+      <c r="AX21" s="1"/>
+    </row>
+    <row r="22" spans="2:50" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
@@ -4244,8 +4595,27 @@
       <c r="AG22" s="4"/>
       <c r="AH22" s="5"/>
       <c r="AI22" s="1"/>
-    </row>
-    <row r="23" spans="2:35" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AJ22" s="1"/>
+      <c r="AK22" s="66" t="s">
+        <v>66</v>
+      </c>
+      <c r="AL22" s="8"/>
+      <c r="AM22" s="4"/>
+      <c r="AN22" s="5"/>
+      <c r="AO22" s="1"/>
+      <c r="AP22" s="1"/>
+      <c r="AQ22" s="66" t="s">
+        <v>66</v>
+      </c>
+      <c r="AR22" s="8"/>
+      <c r="AS22" s="4"/>
+      <c r="AT22" s="5"/>
+      <c r="AU22" s="4"/>
+      <c r="AV22" s="1"/>
+      <c r="AW22" s="1"/>
+      <c r="AX22" s="1"/>
+    </row>
+    <row r="23" spans="2:50" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -4284,8 +4654,31 @@
       </c>
       <c r="AH23" s="5"/>
       <c r="AI23" s="1"/>
-    </row>
-    <row r="24" spans="2:35" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AJ23" s="1"/>
+      <c r="AK23" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="AL23" s="4"/>
+      <c r="AM23" s="59" t="s">
+        <v>90</v>
+      </c>
+      <c r="AN23" s="5"/>
+      <c r="AO23" s="1"/>
+      <c r="AP23" s="1"/>
+      <c r="AQ23" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="AR23" s="4"/>
+      <c r="AS23" s="59" t="s">
+        <v>90</v>
+      </c>
+      <c r="AT23" s="5"/>
+      <c r="AU23" s="5"/>
+      <c r="AV23" s="1"/>
+      <c r="AW23" s="1"/>
+      <c r="AX23" s="1"/>
+    </row>
+    <row r="24" spans="2:50" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
@@ -4322,8 +4715,27 @@
       <c r="AG24" s="1"/>
       <c r="AH24" s="4"/>
       <c r="AI24" s="1"/>
-    </row>
-    <row r="25" spans="2:35" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AJ24" s="1"/>
+      <c r="AK24" s="1"/>
+      <c r="AL24" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AM24" s="1"/>
+      <c r="AN24" s="4"/>
+      <c r="AO24" s="1"/>
+      <c r="AP24" s="1"/>
+      <c r="AQ24" s="1"/>
+      <c r="AR24" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="AS24" s="1"/>
+      <c r="AT24" s="4"/>
+      <c r="AU24" s="1"/>
+      <c r="AV24" s="1"/>
+      <c r="AW24" s="1"/>
+      <c r="AX24" s="1"/>
+    </row>
+    <row r="25" spans="2:50" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
@@ -4362,8 +4774,29 @@
       <c r="AG25" s="1"/>
       <c r="AH25" s="5"/>
       <c r="AI25" s="1"/>
-    </row>
-    <row r="26" spans="2:35" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AJ25" s="1"/>
+      <c r="AK25" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="AL25" s="66" t="s">
+        <v>91</v>
+      </c>
+      <c r="AM25" s="1"/>
+      <c r="AN25" s="5"/>
+      <c r="AO25" s="1"/>
+      <c r="AP25" s="1"/>
+      <c r="AQ25" s="83"/>
+      <c r="AR25" s="66" t="s">
+        <v>91</v>
+      </c>
+      <c r="AS25" s="1"/>
+      <c r="AT25" s="5"/>
+      <c r="AU25" s="1"/>
+      <c r="AV25" s="1"/>
+      <c r="AW25" s="1"/>
+      <c r="AX25" s="1"/>
+    </row>
+    <row r="26" spans="2:50" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
@@ -4400,8 +4833,27 @@
       <c r="AG26" s="4"/>
       <c r="AH26" s="1"/>
       <c r="AI26" s="1"/>
-    </row>
-    <row r="27" spans="2:35" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AJ26" s="1"/>
+      <c r="AK26" s="66" t="s">
+        <v>92</v>
+      </c>
+      <c r="AL26" s="8"/>
+      <c r="AM26" s="4"/>
+      <c r="AN26" s="1"/>
+      <c r="AO26" s="1"/>
+      <c r="AP26" s="1"/>
+      <c r="AQ26" s="84"/>
+      <c r="AR26" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="AS26" s="4"/>
+      <c r="AT26" s="1"/>
+      <c r="AU26" s="1"/>
+      <c r="AV26" s="1"/>
+      <c r="AW26" s="1"/>
+      <c r="AX26" s="1"/>
+    </row>
+    <row r="27" spans="2:50" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
@@ -4438,8 +4890,25 @@
       <c r="AG27" s="1"/>
       <c r="AH27" s="1"/>
       <c r="AI27" s="1"/>
-    </row>
-    <row r="28" spans="2:35" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="AJ27" s="1"/>
+      <c r="AK27" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="AL27" s="4"/>
+      <c r="AM27" s="1"/>
+      <c r="AN27" s="1"/>
+      <c r="AO27" s="1"/>
+      <c r="AP27" s="1"/>
+      <c r="AQ27" s="83"/>
+      <c r="AR27" s="9"/>
+      <c r="AS27" s="1"/>
+      <c r="AT27" s="1"/>
+      <c r="AU27" s="1"/>
+      <c r="AV27" s="1"/>
+      <c r="AW27" s="1"/>
+      <c r="AX27" s="1"/>
+    </row>
+    <row r="28" spans="2:50" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
@@ -4474,6 +4943,21 @@
       <c r="AG28" s="1"/>
       <c r="AH28" s="1"/>
       <c r="AI28" s="1"/>
+      <c r="AJ28" s="1"/>
+      <c r="AK28" s="1"/>
+      <c r="AL28" s="1"/>
+      <c r="AM28" s="1"/>
+      <c r="AN28" s="1"/>
+      <c r="AO28" s="1"/>
+      <c r="AP28" s="1"/>
+      <c r="AQ28" s="1"/>
+      <c r="AR28" s="1"/>
+      <c r="AS28" s="1"/>
+      <c r="AT28" s="1"/>
+      <c r="AU28" s="1"/>
+      <c r="AV28" s="1"/>
+      <c r="AW28" s="1"/>
+      <c r="AX28" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4484,7 +4968,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC68B215-176C-47A9-BC65-E5FAC0AEE706}">
   <dimension ref="B2:U19"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P2" sqref="P2:U19"/>
     </sheetView>
   </sheetViews>
@@ -4872,8 +5356,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7C06664-9D9D-4861-B1E9-94FF6B95C706}">
   <dimension ref="B1:AC37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="Y17" sqref="Y17"/>
+    <sheetView topLeftCell="L1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="R20" sqref="R20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4975,7 +5459,7 @@
     <row r="6" spans="2:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C6" s="1"/>
       <c r="D6" s="6"/>
-      <c r="E6" s="82"/>
+      <c r="E6" s="1"/>
       <c r="F6" s="6">
         <v>1</v>
       </c>
@@ -4985,7 +5469,7 @@
       <c r="J6" s="1"/>
       <c r="L6" s="1"/>
       <c r="M6" s="6"/>
-      <c r="N6" s="82"/>
+      <c r="N6" s="1"/>
       <c r="O6" s="6" t="s">
         <v>109</v>
       </c>
@@ -4995,7 +5479,7 @@
       <c r="S6" s="1"/>
       <c r="U6" s="1"/>
       <c r="V6" s="6"/>
-      <c r="W6" s="82"/>
+      <c r="W6" s="1"/>
       <c r="X6" s="6" t="s">
         <v>110</v>
       </c>
@@ -5008,7 +5492,7 @@
     <row r="7" spans="2:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C7" s="1"/>
       <c r="D7" s="6"/>
-      <c r="E7" s="82"/>
+      <c r="E7" s="1"/>
       <c r="F7" s="11"/>
       <c r="G7" s="5"/>
       <c r="H7" s="1"/>
@@ -5016,7 +5500,7 @@
       <c r="J7" s="1"/>
       <c r="L7" s="1"/>
       <c r="M7" s="6"/>
-      <c r="N7" s="82"/>
+      <c r="N7" s="1"/>
       <c r="O7" s="11"/>
       <c r="P7" s="5"/>
       <c r="Q7" s="1"/>
@@ -5026,7 +5510,7 @@
       <c r="V7" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="W7" s="82"/>
+      <c r="W7" s="1"/>
       <c r="X7" s="11"/>
       <c r="Y7" s="5"/>
       <c r="Z7" s="1"/>
@@ -5367,7 +5851,7 @@
       <c r="X18" s="7"/>
       <c r="Y18" s="1"/>
       <c r="Z18" s="1"/>
-      <c r="AA18" s="84"/>
+      <c r="AA18" s="73"/>
       <c r="AB18" s="1"/>
       <c r="AC18" s="1"/>
     </row>
@@ -5398,7 +5882,7 @@
       </c>
       <c r="Y19" s="4"/>
       <c r="Z19" s="5"/>
-      <c r="AA19" s="84"/>
+      <c r="AA19" s="73"/>
       <c r="AB19" s="1"/>
       <c r="AC19" s="1"/>
     </row>
@@ -5429,7 +5913,7 @@
       <c r="X20" s="1"/>
       <c r="Y20" s="1"/>
       <c r="Z20" s="5"/>
-      <c r="AA20" s="84"/>
+      <c r="AA20" s="73"/>
       <c r="AB20" s="1"/>
       <c r="AC20" s="1"/>
     </row>
@@ -5450,7 +5934,7 @@
       <c r="Q21" s="1"/>
       <c r="R21" s="4"/>
       <c r="S21" s="1"/>
-      <c r="U21" s="82"/>
+      <c r="U21" s="1"/>
       <c r="V21" s="8" t="s">
         <v>111</v>
       </c>
@@ -5458,14 +5942,14 @@
       <c r="X21" s="5"/>
       <c r="Y21" s="1"/>
       <c r="Z21" s="5"/>
-      <c r="AA21" s="84"/>
+      <c r="AA21" s="73"/>
       <c r="AB21" s="1"/>
       <c r="AC21" s="1"/>
     </row>
     <row r="22" spans="3:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C22" s="1"/>
       <c r="D22" s="6"/>
-      <c r="E22" s="82"/>
+      <c r="E22" s="1"/>
       <c r="F22" s="6">
         <v>3</v>
       </c>
@@ -5475,7 +5959,7 @@
       <c r="J22" s="1"/>
       <c r="L22" s="1"/>
       <c r="M22" s="6"/>
-      <c r="N22" s="82"/>
+      <c r="N22" s="1"/>
       <c r="O22" s="6" t="s">
         <v>110</v>
       </c>
@@ -5483,7 +5967,7 @@
       <c r="Q22" s="1"/>
       <c r="R22" s="5"/>
       <c r="S22" s="1"/>
-      <c r="U22" s="82"/>
+      <c r="U22" s="1"/>
       <c r="V22" s="6"/>
       <c r="W22" s="6"/>
       <c r="X22" s="5"/>
@@ -5496,7 +5980,7 @@
     <row r="23" spans="3:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C23" s="1"/>
       <c r="D23" s="6"/>
-      <c r="E23" s="82"/>
+      <c r="E23" s="1"/>
       <c r="F23" s="11"/>
       <c r="G23" s="5"/>
       <c r="H23" s="1"/>
@@ -5504,13 +5988,13 @@
       <c r="J23" s="1"/>
       <c r="L23" s="1"/>
       <c r="M23" s="6"/>
-      <c r="N23" s="82"/>
+      <c r="N23" s="1"/>
       <c r="O23" s="11"/>
       <c r="P23" s="5"/>
       <c r="Q23" s="1"/>
       <c r="R23" s="5"/>
       <c r="S23" s="1"/>
-      <c r="U23" s="82"/>
+      <c r="U23" s="1"/>
       <c r="V23" s="6" t="s">
         <v>111</v>
       </c>
@@ -5541,7 +6025,7 @@
       <c r="Q24" s="1"/>
       <c r="R24" s="5"/>
       <c r="S24" s="1"/>
-      <c r="U24" s="82"/>
+      <c r="U24" s="1"/>
       <c r="V24" s="7"/>
       <c r="W24" s="1"/>
       <c r="X24" s="5"/>
@@ -5572,14 +6056,14 @@
       <c r="Q25" s="5"/>
       <c r="R25" s="5"/>
       <c r="S25" s="1"/>
-      <c r="U25" s="82"/>
+      <c r="U25" s="1"/>
       <c r="V25" s="8" t="s">
         <v>111</v>
       </c>
       <c r="W25" s="4"/>
       <c r="X25" s="6"/>
       <c r="Y25" s="4"/>
-      <c r="Z25" s="82"/>
+      <c r="Z25" s="1"/>
       <c r="AA25" s="14"/>
       <c r="AB25" s="1"/>
       <c r="AC25" s="1"/>
@@ -5605,14 +6089,14 @@
       <c r="Q26" s="5"/>
       <c r="R26" s="5"/>
       <c r="S26" s="1"/>
-      <c r="U26" s="82"/>
-      <c r="V26" s="83"/>
-      <c r="W26" s="83"/>
+      <c r="U26" s="1"/>
+      <c r="V26" s="6"/>
+      <c r="W26" s="6"/>
       <c r="X26" s="8" t="s">
         <v>110</v>
       </c>
       <c r="Y26" s="5"/>
-      <c r="Z26" s="82"/>
+      <c r="Z26" s="1"/>
       <c r="AA26" s="3" t="s">
         <v>109</v>
       </c>
@@ -5636,13 +6120,13 @@
       <c r="Q27" s="5"/>
       <c r="R27" s="5"/>
       <c r="S27" s="1"/>
-      <c r="U27" s="82"/>
-      <c r="V27" s="83"/>
-      <c r="W27" s="82"/>
-      <c r="X27" s="83"/>
-      <c r="Y27" s="82"/>
-      <c r="Z27" s="82"/>
-      <c r="AA27" s="82"/>
+      <c r="U27" s="1"/>
+      <c r="V27" s="6"/>
+      <c r="W27" s="1"/>
+      <c r="X27" s="6"/>
+      <c r="Y27" s="1"/>
+      <c r="Z27" s="1"/>
+      <c r="AA27" s="1"/>
       <c r="AB27" s="1"/>
       <c r="AC27" s="1"/>
     </row>
@@ -5667,13 +6151,13 @@
       <c r="Q28" s="5"/>
       <c r="R28" s="5"/>
       <c r="S28" s="1"/>
-      <c r="U28" s="82"/>
-      <c r="V28" s="83"/>
-      <c r="W28" s="82"/>
-      <c r="X28" s="83"/>
-      <c r="Y28" s="82"/>
-      <c r="Z28" s="82"/>
-      <c r="AA28" s="82"/>
+      <c r="U28" s="1"/>
+      <c r="V28" s="6"/>
+      <c r="W28" s="1"/>
+      <c r="X28" s="6"/>
+      <c r="Y28" s="1"/>
+      <c r="Z28" s="1"/>
+      <c r="AA28" s="1"/>
       <c r="AB28" s="1"/>
       <c r="AC28" s="1"/>
     </row>
@@ -5694,12 +6178,12 @@
       <c r="Q29" s="4"/>
       <c r="R29" s="1"/>
       <c r="S29" s="1"/>
-      <c r="U29" s="82"/>
-      <c r="V29" s="83"/>
-      <c r="W29" s="82"/>
-      <c r="X29" s="83"/>
-      <c r="Y29" s="82"/>
-      <c r="Z29" s="82"/>
+      <c r="U29" s="1"/>
+      <c r="V29" s="6"/>
+      <c r="W29" s="1"/>
+      <c r="X29" s="6"/>
+      <c r="Y29" s="1"/>
+      <c r="Z29" s="1"/>
       <c r="AA29" s="1"/>
       <c r="AB29" s="1"/>
       <c r="AC29" s="1"/>
@@ -5707,7 +6191,7 @@
     <row r="30" spans="3:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C30" s="1"/>
       <c r="D30" s="6"/>
-      <c r="E30" s="82"/>
+      <c r="E30" s="1"/>
       <c r="F30" s="6">
         <v>2</v>
       </c>
@@ -5717,7 +6201,7 @@
       <c r="J30" s="1"/>
       <c r="L30" s="1"/>
       <c r="M30" s="6"/>
-      <c r="N30" s="82"/>
+      <c r="N30" s="1"/>
       <c r="O30" s="6" t="s">
         <v>110</v>
       </c>
@@ -5725,12 +6209,12 @@
       <c r="Q30" s="5"/>
       <c r="R30" s="1"/>
       <c r="S30" s="1"/>
-      <c r="U30" s="82"/>
-      <c r="V30" s="83"/>
-      <c r="W30" s="82"/>
-      <c r="X30" s="83"/>
-      <c r="Y30" s="82"/>
-      <c r="Z30" s="82"/>
+      <c r="U30" s="1"/>
+      <c r="V30" s="6"/>
+      <c r="W30" s="1"/>
+      <c r="X30" s="6"/>
+      <c r="Y30" s="1"/>
+      <c r="Z30" s="1"/>
       <c r="AA30" s="1"/>
       <c r="AB30" s="1"/>
       <c r="AC30" s="1"/>
@@ -5738,7 +6222,7 @@
     <row r="31" spans="3:29" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="C31" s="1"/>
       <c r="D31" s="6"/>
-      <c r="E31" s="82"/>
+      <c r="E31" s="1"/>
       <c r="F31" s="11"/>
       <c r="G31" s="5"/>
       <c r="H31" s="5"/>
@@ -5746,18 +6230,18 @@
       <c r="J31" s="1"/>
       <c r="L31" s="1"/>
       <c r="M31" s="6"/>
-      <c r="N31" s="82"/>
+      <c r="N31" s="1"/>
       <c r="O31" s="11"/>
       <c r="P31" s="5"/>
       <c r="Q31" s="5"/>
       <c r="R31" s="1"/>
       <c r="S31" s="1"/>
-      <c r="U31" s="82"/>
-      <c r="V31" s="83"/>
-      <c r="W31" s="82"/>
-      <c r="X31" s="83"/>
-      <c r="Y31" s="82"/>
-      <c r="Z31" s="82"/>
+      <c r="U31" s="1"/>
+      <c r="V31" s="6"/>
+      <c r="W31" s="1"/>
+      <c r="X31" s="6"/>
+      <c r="Y31" s="1"/>
+      <c r="Z31" s="1"/>
       <c r="AA31" s="1"/>
       <c r="AB31" s="1"/>
       <c r="AC31" s="1"/>
@@ -5779,12 +6263,12 @@
       <c r="Q32" s="5"/>
       <c r="R32" s="1"/>
       <c r="S32" s="1"/>
-      <c r="U32" s="82"/>
-      <c r="V32" s="83"/>
-      <c r="W32" s="83"/>
-      <c r="X32" s="83"/>
-      <c r="Y32" s="82"/>
-      <c r="Z32" s="82"/>
+      <c r="U32" s="1"/>
+      <c r="V32" s="6"/>
+      <c r="W32" s="6"/>
+      <c r="X32" s="6"/>
+      <c r="Y32" s="1"/>
+      <c r="Z32" s="1"/>
       <c r="AA32" s="1"/>
       <c r="AB32" s="1"/>
       <c r="AC32" s="1"/>
@@ -5810,12 +6294,12 @@
       <c r="Q33" s="1"/>
       <c r="R33" s="1"/>
       <c r="S33" s="1"/>
-      <c r="U33" s="82"/>
-      <c r="V33" s="83"/>
-      <c r="W33" s="83"/>
-      <c r="X33" s="83"/>
-      <c r="Y33" s="82"/>
-      <c r="Z33" s="82"/>
+      <c r="U33" s="1"/>
+      <c r="V33" s="6"/>
+      <c r="W33" s="6"/>
+      <c r="X33" s="6"/>
+      <c r="Y33" s="1"/>
+      <c r="Z33" s="1"/>
       <c r="AA33" s="1"/>
       <c r="AB33" s="1"/>
       <c r="AC33" s="1"/>
@@ -5841,12 +6325,12 @@
       <c r="Q34" s="1"/>
       <c r="R34" s="1"/>
       <c r="S34" s="1"/>
-      <c r="U34" s="82"/>
-      <c r="V34" s="83"/>
-      <c r="W34" s="83"/>
-      <c r="X34" s="83"/>
-      <c r="Y34" s="82"/>
-      <c r="Z34" s="82"/>
+      <c r="U34" s="1"/>
+      <c r="V34" s="6"/>
+      <c r="W34" s="6"/>
+      <c r="X34" s="6"/>
+      <c r="Y34" s="1"/>
+      <c r="Z34" s="1"/>
       <c r="AA34" s="1"/>
       <c r="AB34" s="1"/>
       <c r="AC34" s="1"/>
@@ -5868,12 +6352,12 @@
       <c r="Q35" s="1"/>
       <c r="R35" s="1"/>
       <c r="S35" s="1"/>
-      <c r="U35" s="82"/>
-      <c r="V35" s="83"/>
-      <c r="W35" s="82"/>
-      <c r="X35" s="83"/>
-      <c r="Y35" s="82"/>
-      <c r="Z35" s="82"/>
+      <c r="U35" s="1"/>
+      <c r="V35" s="6"/>
+      <c r="W35" s="1"/>
+      <c r="X35" s="6"/>
+      <c r="Y35" s="1"/>
+      <c r="Z35" s="1"/>
       <c r="AA35" s="1"/>
       <c r="AB35" s="1"/>
       <c r="AC35" s="1"/>
@@ -5899,12 +6383,12 @@
       <c r="Q36" s="1"/>
       <c r="R36" s="1"/>
       <c r="S36" s="1"/>
-      <c r="U36" s="82"/>
-      <c r="V36" s="83"/>
-      <c r="W36" s="82"/>
-      <c r="X36" s="83"/>
-      <c r="Y36" s="82"/>
-      <c r="Z36" s="82"/>
+      <c r="U36" s="1"/>
+      <c r="V36" s="6"/>
+      <c r="W36" s="1"/>
+      <c r="X36" s="6"/>
+      <c r="Y36" s="1"/>
+      <c r="Z36" s="1"/>
       <c r="AA36" s="1"/>
       <c r="AB36" s="1"/>
       <c r="AC36" s="1"/>
@@ -5926,12 +6410,12 @@
       <c r="Q37" s="1"/>
       <c r="R37" s="1"/>
       <c r="S37" s="1"/>
-      <c r="U37" s="82"/>
-      <c r="V37" s="83"/>
-      <c r="W37" s="82"/>
-      <c r="X37" s="83"/>
-      <c r="Y37" s="82"/>
-      <c r="Z37" s="82"/>
+      <c r="U37" s="1"/>
+      <c r="V37" s="6"/>
+      <c r="W37" s="1"/>
+      <c r="X37" s="6"/>
+      <c r="Y37" s="1"/>
+      <c r="Z37" s="1"/>
       <c r="AA37" s="1"/>
       <c r="AB37" s="1"/>
       <c r="AC37" s="1"/>
@@ -5966,16 +6450,16 @@
     </row>
     <row r="5" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C5" s="1"/>
-      <c r="D5" s="80" t="s">
+      <c r="D5" s="81" t="s">
         <v>96</v>
       </c>
-      <c r="E5" s="81"/>
+      <c r="E5" s="82"/>
       <c r="F5" s="67"/>
       <c r="G5" s="6"/>
-      <c r="H5" s="80" t="s">
+      <c r="H5" s="81" t="s">
         <v>95</v>
       </c>
-      <c r="I5" s="81"/>
+      <c r="I5" s="82"/>
       <c r="J5" s="1"/>
     </row>
     <row r="6" spans="3:10" x14ac:dyDescent="0.3">
@@ -10258,7 +10742,7 @@
         <v>18</v>
       </c>
       <c r="C8" s="4"/>
-      <c r="D8" s="73"/>
+      <c r="D8" s="74"/>
       <c r="E8" s="1"/>
       <c r="F8" s="4"/>
       <c r="G8" s="5"/>
@@ -10266,7 +10750,7 @@
     <row r="9" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
-      <c r="D9" s="73"/>
+      <c r="D9" s="74"/>
       <c r="E9" s="8" t="s">
         <v>16</v>
       </c>
@@ -10300,7 +10784,7 @@
         <v>20</v>
       </c>
       <c r="C12" s="4"/>
-      <c r="D12" s="73"/>
+      <c r="D12" s="74"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="4"/>
@@ -10308,7 +10792,7 @@
     <row r="13" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
-      <c r="D13" s="73"/>
+      <c r="D13" s="74"/>
       <c r="E13" s="1" t="s">
         <v>15</v>
       </c>
@@ -10342,7 +10826,7 @@
         <v>22</v>
       </c>
       <c r="C16" s="4"/>
-      <c r="D16" s="73"/>
+      <c r="D16" s="74"/>
       <c r="E16" s="1"/>
       <c r="F16" s="4"/>
       <c r="G16" s="1"/>
@@ -10350,7 +10834,7 @@
     <row r="17" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
-      <c r="D17" s="73"/>
+      <c r="D17" s="74"/>
       <c r="E17" s="1" t="s">
         <v>14</v>
       </c>
@@ -10446,7 +10930,7 @@
         <v>24</v>
       </c>
       <c r="C8" s="4"/>
-      <c r="D8" s="73"/>
+      <c r="D8" s="74"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
@@ -10456,7 +10940,7 @@
     <row r="9" spans="2:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
-      <c r="D9" s="73"/>
+      <c r="D9" s="74"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="8" t="s">
@@ -10471,8 +10955,8 @@
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="78"/>
-      <c r="F10" s="79"/>
+      <c r="E10" s="80"/>
+      <c r="F10" s="75"/>
       <c r="G10" s="6"/>
       <c r="H10" s="1"/>
       <c r="I10" s="5"/>
@@ -10481,8 +10965,8 @@
       <c r="B11" s="76"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="78"/>
-      <c r="F11" s="79"/>
+      <c r="E11" s="80"/>
+      <c r="F11" s="75"/>
       <c r="G11" s="6"/>
       <c r="H11" s="1"/>
       <c r="I11" s="5"/>
@@ -10491,7 +10975,7 @@
       <c r="B12" s="77"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="79"/>
+      <c r="E12" s="75"/>
       <c r="F12" s="1"/>
       <c r="G12" s="6"/>
       <c r="H12" s="1"/>
@@ -10503,33 +10987,33 @@
         <v>29</v>
       </c>
       <c r="D13" s="1"/>
-      <c r="E13" s="79"/>
+      <c r="E13" s="75"/>
       <c r="F13" s="1"/>
       <c r="G13" s="6"/>
       <c r="H13" s="1"/>
-      <c r="I13" s="74" t="s">
+      <c r="I13" s="78" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="14" spans="2:9" ht="4.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="14"/>
       <c r="C14" s="76"/>
-      <c r="D14" s="79"/>
-      <c r="E14" s="78"/>
+      <c r="D14" s="75"/>
+      <c r="E14" s="80"/>
       <c r="F14" s="1"/>
       <c r="G14" s="6"/>
       <c r="H14" s="1"/>
-      <c r="I14" s="74"/>
+      <c r="I14" s="78"/>
     </row>
     <row r="15" spans="2:9" ht="4.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="18"/>
       <c r="C15" s="77"/>
-      <c r="D15" s="79"/>
-      <c r="E15" s="78"/>
+      <c r="D15" s="75"/>
+      <c r="E15" s="80"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
-      <c r="I15" s="75"/>
+      <c r="I15" s="79"/>
     </row>
     <row r="16" spans="2:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="8" t="s">
@@ -10538,7 +11022,7 @@
       <c r="C16" s="9"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
-      <c r="F16" s="73"/>
+      <c r="F16" s="74"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="4"/>
@@ -10548,7 +11032,7 @@
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
-      <c r="F17" s="73"/>
+      <c r="F17" s="74"/>
       <c r="G17" s="1" t="s">
         <v>30</v>
       </c>
@@ -10586,9 +11070,9 @@
         <v>27</v>
       </c>
       <c r="C20" s="4"/>
-      <c r="D20" s="73"/>
-      <c r="E20" s="73"/>
-      <c r="F20" s="73"/>
+      <c r="D20" s="74"/>
+      <c r="E20" s="74"/>
+      <c r="F20" s="74"/>
       <c r="G20" s="1"/>
       <c r="H20" s="4"/>
       <c r="I20" s="1"/>
@@ -10596,9 +11080,9 @@
     <row r="21" spans="2:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
-      <c r="D21" s="73"/>
-      <c r="E21" s="73"/>
-      <c r="F21" s="73"/>
+      <c r="D21" s="74"/>
+      <c r="E21" s="74"/>
+      <c r="F21" s="74"/>
       <c r="G21" s="1" t="s">
         <v>2</v>
       </c>
@@ -10617,17 +11101,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="I13:I15"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="E14:E15"/>
     <mergeCell ref="D20:F21"/>
     <mergeCell ref="F16:F17"/>
     <mergeCell ref="F10:F11"/>
     <mergeCell ref="C13:C15"/>
     <mergeCell ref="D14:D15"/>
     <mergeCell ref="E12:E13"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="I13:I15"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="E14:E15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated simple multibrackets with proper respectfulness
</commit_message>
<xml_diff>
--- a/thesis-tex/images/Brackets/Brackets.xlsx
+++ b/thesis-tex/images/Brackets/Brackets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leofr\Documents\LeoWork\School\04College\17Senior\thesis\thesis-tex\images\Brackets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80185915-6F29-49BF-8F58-2B640A94ACEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3674D2C3-9098-471A-8B47-D9958776E263}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="9" activeTab="15" xr2:uid="{503DA620-194E-433E-B5EB-5393E7537419}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="8" activeTab="10" xr2:uid="{503DA620-194E-433E-B5EB-5393E7537419}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,6 +32,7 @@
     <sheet name="Sheet8" sheetId="17" r:id="rId17"/>
     <sheet name="Sheet16" sheetId="18" r:id="rId18"/>
     <sheet name="Sheet18" sheetId="20" r:id="rId19"/>
+    <sheet name="Sheet19" sheetId="21" r:id="rId20"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -54,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="116">
   <si>
     <t>Georgia</t>
   </si>
@@ -868,7 +869,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -986,7 +987,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -995,13 +999,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1012,9 +1013,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2073,8 +2071,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C071CB8-4A62-48A5-9C91-383608FE5F7C}">
   <dimension ref="A5:R18"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="S16" sqref="S16"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2304,7 +2302,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D228CAD8-B85C-426E-AD63-CE67C9560447}">
   <dimension ref="B5:Q29"/>
   <sheetViews>
-    <sheetView topLeftCell="AD1" workbookViewId="0">
+    <sheetView topLeftCell="T1" workbookViewId="0">
       <selection activeCell="T15" sqref="T15"/>
     </sheetView>
   </sheetViews>
@@ -3222,7 +3220,7 @@
     </row>
     <row r="10" spans="3:7" ht="7.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C10" s="1"/>
-      <c r="D10" s="76" t="s">
+      <c r="D10" s="77" t="s">
         <v>49</v>
       </c>
       <c r="E10" s="1"/>
@@ -3231,7 +3229,7 @@
     </row>
     <row r="11" spans="3:7" ht="7.8" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C11" s="64"/>
-      <c r="D11" s="77"/>
+      <c r="D11" s="78"/>
       <c r="E11" s="1"/>
       <c r="F11" s="20"/>
       <c r="G11" s="1"/>
@@ -3277,7 +3275,7 @@
     </row>
     <row r="17" spans="3:7" ht="7.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C17" s="1"/>
-      <c r="D17" s="76" t="s">
+      <c r="D17" s="77" t="s">
         <v>53</v>
       </c>
       <c r="E17" s="1"/>
@@ -3286,7 +3284,7 @@
     </row>
     <row r="18" spans="3:7" ht="7.8" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C18" s="64"/>
-      <c r="D18" s="77"/>
+      <c r="D18" s="78"/>
       <c r="E18" s="1"/>
       <c r="F18" s="20"/>
       <c r="G18" s="1"/>
@@ -3328,7 +3326,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BF5E35F-6BAF-409B-A5CF-ACCF63F9A711}">
   <dimension ref="B4:AX28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -4785,7 +4783,7 @@
       <c r="AN25" s="5"/>
       <c r="AO25" s="1"/>
       <c r="AP25" s="1"/>
-      <c r="AQ25" s="83"/>
+      <c r="AQ25" s="6"/>
       <c r="AR25" s="66" t="s">
         <v>91</v>
       </c>
@@ -4842,7 +4840,7 @@
       <c r="AN26" s="1"/>
       <c r="AO26" s="1"/>
       <c r="AP26" s="1"/>
-      <c r="AQ26" s="84"/>
+      <c r="AQ26" s="59"/>
       <c r="AR26" s="8" t="s">
         <v>60</v>
       </c>
@@ -4899,7 +4897,7 @@
       <c r="AN27" s="1"/>
       <c r="AO27" s="1"/>
       <c r="AP27" s="1"/>
-      <c r="AQ27" s="83"/>
+      <c r="AQ27" s="6"/>
       <c r="AR27" s="9"/>
       <c r="AS27" s="1"/>
       <c r="AT27" s="1"/>
@@ -5357,7 +5355,7 @@
   <dimension ref="B1:AC37"/>
   <sheetViews>
     <sheetView topLeftCell="L1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="R20" sqref="R20"/>
+      <selection activeCell="R9" sqref="R9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6429,8 +6427,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D84D55B-86DB-41A7-86B6-8D3E6C4FEE99}">
   <dimension ref="C4:J29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:J1048576"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22:G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6982,6 +6980,583 @@
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A138887D-E83F-4832-AC66-DEE1E0C0D3AC}">
+  <dimension ref="A4:O33"/>
+  <sheetViews>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="S23" sqref="S23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+    </row>
+    <row r="6" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+    </row>
+    <row r="7" spans="1:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D7" s="7"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="J7" s="7"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+    </row>
+    <row r="8" spans="1:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="I8" s="7"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+    </row>
+    <row r="9" spans="1:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="D9" s="4"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+    </row>
+    <row r="10" spans="1:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="I10" s="4"/>
+      <c r="J10" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="K10" s="1"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+    </row>
+    <row r="11" spans="1:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D11" s="7"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="J11" s="7"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+    </row>
+    <row r="12" spans="1:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C12" s="7"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+    </row>
+    <row r="13" spans="1:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="1"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="J13" s="4"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+    </row>
+    <row r="14" spans="1:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="1"/>
+      <c r="B14" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="C14" s="4"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+    </row>
+    <row r="15" spans="1:15" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+    </row>
+    <row r="20" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+    </row>
+    <row r="21" spans="1:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="83"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+    </row>
+    <row r="22" spans="1:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="D22" s="7"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="83"/>
+      <c r="I22" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="J22" s="4"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+    </row>
+    <row r="23" spans="1:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="83"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
+    </row>
+    <row r="24" spans="1:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="D24" s="4"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="I24" s="6"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="5"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
+    </row>
+    <row r="25" spans="1:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="E25" s="1"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="4"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
+      <c r="N25" s="1"/>
+      <c r="O25" s="1"/>
+    </row>
+    <row r="26" spans="1:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="D26" s="7"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="I26" s="4"/>
+      <c r="J26" s="5"/>
+      <c r="K26" s="5"/>
+      <c r="L26" s="1"/>
+      <c r="M26" s="1"/>
+      <c r="N26" s="1"/>
+      <c r="O26" s="1"/>
+    </row>
+    <row r="27" spans="1:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="5"/>
+      <c r="L27" s="1"/>
+      <c r="M27" s="1"/>
+      <c r="N27" s="1"/>
+      <c r="O27" s="1"/>
+    </row>
+    <row r="28" spans="1:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="D28" s="4"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="I28" s="1"/>
+      <c r="J28" s="4"/>
+      <c r="K28" s="1"/>
+      <c r="L28" s="1"/>
+      <c r="M28" s="1"/>
+      <c r="N28" s="1"/>
+      <c r="O28" s="1"/>
+    </row>
+    <row r="29" spans="1:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="7"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="5"/>
+      <c r="K29" s="1"/>
+      <c r="L29" s="1"/>
+      <c r="M29" s="1"/>
+      <c r="N29" s="1"/>
+      <c r="O29" s="1"/>
+    </row>
+    <row r="30" spans="1:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="I30" s="4"/>
+      <c r="J30" s="1"/>
+      <c r="K30" s="1"/>
+      <c r="L30" s="1"/>
+      <c r="M30" s="1"/>
+      <c r="N30" s="1"/>
+      <c r="O30" s="1"/>
+    </row>
+    <row r="31" spans="1:15" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
+      <c r="K31" s="1"/>
+      <c r="L31" s="1"/>
+      <c r="M31" s="1"/>
+      <c r="N31" s="1"/>
+      <c r="O31" s="1"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
+      <c r="K32" s="1"/>
+      <c r="L32" s="1"/>
+      <c r="M32" s="1"/>
+      <c r="N32" s="1"/>
+      <c r="O32" s="1"/>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+      <c r="K33" s="1"/>
+      <c r="L33" s="1"/>
+      <c r="M33" s="1"/>
+      <c r="N33" s="1"/>
+      <c r="O33" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10864,7 +11439,7 @@
   <dimension ref="B4:I22"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16:D17"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10950,32 +11525,32 @@
       <c r="I9" s="5"/>
     </row>
     <row r="10" spans="2:9" ht="4.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="76" t="s">
+      <c r="B10" s="77" t="s">
         <v>25</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="80"/>
-      <c r="F10" s="75"/>
+      <c r="E10" s="79"/>
+      <c r="F10" s="80"/>
       <c r="G10" s="6"/>
       <c r="H10" s="1"/>
       <c r="I10" s="5"/>
     </row>
     <row r="11" spans="2:9" ht="4.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="76"/>
+      <c r="B11" s="77"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="80"/>
-      <c r="F11" s="75"/>
+      <c r="E11" s="79"/>
+      <c r="F11" s="80"/>
       <c r="G11" s="6"/>
       <c r="H11" s="1"/>
       <c r="I11" s="5"/>
     </row>
     <row r="12" spans="2:9" ht="4.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="77"/>
+      <c r="B12" s="78"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="75"/>
+      <c r="E12" s="80"/>
       <c r="F12" s="1"/>
       <c r="G12" s="6"/>
       <c r="H12" s="1"/>
@@ -10983,37 +11558,37 @@
     </row>
     <row r="13" spans="2:9" ht="4.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B13" s="2"/>
-      <c r="C13" s="76" t="s">
+      <c r="C13" s="77" t="s">
         <v>29</v>
       </c>
       <c r="D13" s="1"/>
-      <c r="E13" s="75"/>
+      <c r="E13" s="80"/>
       <c r="F13" s="1"/>
       <c r="G13" s="6"/>
       <c r="H13" s="1"/>
-      <c r="I13" s="78" t="s">
+      <c r="I13" s="75" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="14" spans="2:9" ht="4.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="14"/>
-      <c r="C14" s="76"/>
-      <c r="D14" s="75"/>
-      <c r="E14" s="80"/>
+      <c r="C14" s="77"/>
+      <c r="D14" s="80"/>
+      <c r="E14" s="79"/>
       <c r="F14" s="1"/>
       <c r="G14" s="6"/>
       <c r="H14" s="1"/>
-      <c r="I14" s="78"/>
+      <c r="I14" s="75"/>
     </row>
     <row r="15" spans="2:9" ht="4.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="18"/>
-      <c r="C15" s="77"/>
-      <c r="D15" s="75"/>
-      <c r="E15" s="80"/>
+      <c r="C15" s="78"/>
+      <c r="D15" s="80"/>
+      <c r="E15" s="79"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
-      <c r="I15" s="79"/>
+      <c r="I15" s="76"/>
     </row>
     <row r="16" spans="2:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="8" t="s">
@@ -11101,17 +11676,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="I13:I15"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="E14:E15"/>
     <mergeCell ref="D20:F21"/>
     <mergeCell ref="F16:F17"/>
     <mergeCell ref="F10:F11"/>
     <mergeCell ref="C13:C15"/>
     <mergeCell ref="D14:D15"/>
     <mergeCell ref="E12:E13"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="I13:I15"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="E14:E15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Starting to redevelop semibrackets.tex
</commit_message>
<xml_diff>
--- a/thesis-tex/images/Brackets/Brackets.xlsx
+++ b/thesis-tex/images/Brackets/Brackets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leofr\Documents\LeoWork\School\04College\17Senior\thesis\thesis-tex\images\Brackets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3674D2C3-9098-471A-8B47-D9958776E263}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D468E4AF-7A45-4F4F-A921-D57AD52A75E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="8" activeTab="10" xr2:uid="{503DA620-194E-433E-B5EB-5393E7537419}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="9" activeTab="15" xr2:uid="{503DA620-194E-433E-B5EB-5393E7537419}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="116">
   <si>
     <t>Georgia</t>
   </si>
@@ -869,7 +869,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -987,10 +987,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -999,10 +996,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1011,8 +1011,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2071,7 +2072,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C071CB8-4A62-48A5-9C91-383608FE5F7C}">
   <dimension ref="A5:R18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView topLeftCell="BA1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
@@ -3220,7 +3221,7 @@
     </row>
     <row r="10" spans="3:7" ht="7.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C10" s="1"/>
-      <c r="D10" s="77" t="s">
+      <c r="D10" s="76" t="s">
         <v>49</v>
       </c>
       <c r="E10" s="1"/>
@@ -3229,7 +3230,7 @@
     </row>
     <row r="11" spans="3:7" ht="7.8" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C11" s="64"/>
-      <c r="D11" s="78"/>
+      <c r="D11" s="77"/>
       <c r="E11" s="1"/>
       <c r="F11" s="20"/>
       <c r="G11" s="1"/>
@@ -3275,7 +3276,7 @@
     </row>
     <row r="17" spans="3:7" ht="7.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C17" s="1"/>
-      <c r="D17" s="77" t="s">
+      <c r="D17" s="76" t="s">
         <v>53</v>
       </c>
       <c r="E17" s="1"/>
@@ -3284,7 +3285,7 @@
     </row>
     <row r="18" spans="3:7" ht="7.8" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C18" s="64"/>
-      <c r="D18" s="78"/>
+      <c r="D18" s="77"/>
       <c r="E18" s="1"/>
       <c r="F18" s="20"/>
       <c r="G18" s="1"/>
@@ -3324,10 +3325,10 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BF5E35F-6BAF-409B-A5CF-ACCF63F9A711}">
-  <dimension ref="B4:AX28"/>
+  <dimension ref="B4:BI28"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="XEH2" workbookViewId="0">
+      <selection activeCell="XFD19" sqref="XFD19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3338,7 +3339,7 @@
     <col min="9" max="10" width="10.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:50" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:61" x14ac:dyDescent="0.3">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -3388,8 +3389,19 @@
       <c r="AV4" s="1"/>
       <c r="AW4" s="1"/>
       <c r="AX4" s="1"/>
-    </row>
-    <row r="5" spans="2:50" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AY4" s="1"/>
+      <c r="AZ4" s="1"/>
+      <c r="BA4" s="1"/>
+      <c r="BB4" s="1"/>
+      <c r="BC4" s="1"/>
+      <c r="BD4" s="1"/>
+      <c r="BE4" s="1"/>
+      <c r="BF4" s="1"/>
+      <c r="BG4" s="1"/>
+      <c r="BH4" s="1"/>
+      <c r="BI4" s="1"/>
+    </row>
+    <row r="5" spans="2:61" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="1"/>
       <c r="C5" s="6">
         <v>1</v>
@@ -3453,10 +3465,25 @@
       <c r="AT5" s="1"/>
       <c r="AU5" s="1"/>
       <c r="AV5" s="1"/>
-      <c r="AW5" s="1"/>
+      <c r="AW5" s="6">
+        <v>1</v>
+      </c>
       <c r="AX5" s="1"/>
-    </row>
-    <row r="6" spans="2:50" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AY5" s="1"/>
+      <c r="AZ5" s="1"/>
+      <c r="BA5" s="1"/>
+      <c r="BB5" s="1"/>
+      <c r="BC5" s="1"/>
+      <c r="BD5" s="6">
+        <v>1</v>
+      </c>
+      <c r="BE5" s="1"/>
+      <c r="BF5" s="1"/>
+      <c r="BG5" s="1"/>
+      <c r="BH5" s="1"/>
+      <c r="BI5" s="1"/>
+    </row>
+    <row r="6" spans="2:61" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="1"/>
       <c r="C6" s="66" t="s">
         <v>59</v>
@@ -3520,10 +3547,25 @@
       <c r="AT6" s="1"/>
       <c r="AU6" s="1"/>
       <c r="AV6" s="1"/>
-      <c r="AW6" s="1"/>
+      <c r="AW6" s="66" t="s">
+        <v>59</v>
+      </c>
       <c r="AX6" s="1"/>
-    </row>
-    <row r="7" spans="2:50" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AY6" s="1"/>
+      <c r="AZ6" s="1"/>
+      <c r="BA6" s="1"/>
+      <c r="BB6" s="1"/>
+      <c r="BC6" s="1"/>
+      <c r="BD6" s="66" t="s">
+        <v>59</v>
+      </c>
+      <c r="BE6" s="1"/>
+      <c r="BF6" s="1"/>
+      <c r="BG6" s="1"/>
+      <c r="BH6" s="1"/>
+      <c r="BI6" s="1"/>
+    </row>
+    <row r="7" spans="2:61" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="1"/>
       <c r="C7" s="8">
         <v>8</v>
@@ -3587,10 +3629,25 @@
       <c r="AT7" s="1"/>
       <c r="AU7" s="1"/>
       <c r="AV7" s="1"/>
-      <c r="AW7" s="1"/>
-      <c r="AX7" s="1"/>
-    </row>
-    <row r="8" spans="2:50" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AW7" s="8">
+        <v>8</v>
+      </c>
+      <c r="AX7" s="4"/>
+      <c r="AY7" s="5"/>
+      <c r="AZ7" s="1"/>
+      <c r="BA7" s="1"/>
+      <c r="BB7" s="1"/>
+      <c r="BC7" s="1"/>
+      <c r="BD7" s="8">
+        <v>8</v>
+      </c>
+      <c r="BE7" s="4"/>
+      <c r="BF7" s="5"/>
+      <c r="BG7" s="1"/>
+      <c r="BH7" s="1"/>
+      <c r="BI7" s="1"/>
+    </row>
+    <row r="8" spans="2:61" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="1"/>
       <c r="C8" s="6"/>
       <c r="D8" s="59" t="s">
@@ -3654,10 +3711,25 @@
       <c r="AT8" s="1"/>
       <c r="AU8" s="1"/>
       <c r="AV8" s="1"/>
-      <c r="AW8" s="1"/>
-      <c r="AX8" s="1"/>
-    </row>
-    <row r="9" spans="2:50" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AW8" s="6"/>
+      <c r="AX8" s="59" t="s">
+        <v>63</v>
+      </c>
+      <c r="AY8" s="5"/>
+      <c r="AZ8" s="1"/>
+      <c r="BA8" s="1"/>
+      <c r="BB8" s="1"/>
+      <c r="BC8" s="1"/>
+      <c r="BD8" s="6"/>
+      <c r="BE8" s="59" t="s">
+        <v>63</v>
+      </c>
+      <c r="BF8" s="5"/>
+      <c r="BG8" s="1"/>
+      <c r="BH8" s="1"/>
+      <c r="BI8" s="1"/>
+    </row>
+    <row r="9" spans="2:61" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="1"/>
       <c r="C9" s="6">
         <v>4</v>
@@ -3721,10 +3793,25 @@
       <c r="AT9" s="1"/>
       <c r="AU9" s="1"/>
       <c r="AV9" s="1"/>
-      <c r="AW9" s="1"/>
+      <c r="AW9" s="6">
+        <v>4</v>
+      </c>
       <c r="AX9" s="1"/>
-    </row>
-    <row r="10" spans="2:50" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AY9" s="4"/>
+      <c r="AZ9" s="5"/>
+      <c r="BA9" s="1"/>
+      <c r="BB9" s="1"/>
+      <c r="BC9" s="1"/>
+      <c r="BD9" s="6">
+        <v>4</v>
+      </c>
+      <c r="BE9" s="1"/>
+      <c r="BF9" s="4"/>
+      <c r="BG9" s="1"/>
+      <c r="BH9" s="1"/>
+      <c r="BI9" s="1"/>
+    </row>
+    <row r="10" spans="2:61" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="1"/>
       <c r="C10" s="66" t="s">
         <v>60</v>
@@ -3788,10 +3875,25 @@
       <c r="AT10" s="1"/>
       <c r="AU10" s="1"/>
       <c r="AV10" s="1"/>
-      <c r="AW10" s="1"/>
+      <c r="AW10" s="66" t="s">
+        <v>60</v>
+      </c>
       <c r="AX10" s="1"/>
-    </row>
-    <row r="11" spans="2:50" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AY10" s="5"/>
+      <c r="AZ10" s="5"/>
+      <c r="BA10" s="1"/>
+      <c r="BB10" s="1"/>
+      <c r="BC10" s="1"/>
+      <c r="BD10" s="66" t="s">
+        <v>60</v>
+      </c>
+      <c r="BE10" s="1"/>
+      <c r="BF10" s="5"/>
+      <c r="BG10" s="1"/>
+      <c r="BH10" s="1"/>
+      <c r="BI10" s="1"/>
+    </row>
+    <row r="11" spans="2:61" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="1"/>
       <c r="C11" s="8">
         <v>5</v>
@@ -3855,10 +3957,25 @@
       <c r="AT11" s="1"/>
       <c r="AU11" s="1"/>
       <c r="AV11" s="1"/>
-      <c r="AW11" s="1"/>
-      <c r="AX11" s="1"/>
-    </row>
-    <row r="12" spans="2:50" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AW11" s="8">
+        <v>5</v>
+      </c>
+      <c r="AX11" s="4"/>
+      <c r="AY11" s="1"/>
+      <c r="AZ11" s="5"/>
+      <c r="BA11" s="1"/>
+      <c r="BB11" s="1"/>
+      <c r="BC11" s="1"/>
+      <c r="BD11" s="8">
+        <v>5</v>
+      </c>
+      <c r="BE11" s="4"/>
+      <c r="BF11" s="1"/>
+      <c r="BG11" s="1"/>
+      <c r="BH11" s="1"/>
+      <c r="BI11" s="1"/>
+    </row>
+    <row r="12" spans="2:61" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="1"/>
       <c r="C12" s="6"/>
       <c r="D12" s="1"/>
@@ -3922,10 +4039,23 @@
       <c r="AT12" s="1"/>
       <c r="AU12" s="1"/>
       <c r="AV12" s="1"/>
-      <c r="AW12" s="1"/>
+      <c r="AW12" s="6"/>
       <c r="AX12" s="1"/>
-    </row>
-    <row r="13" spans="2:50" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AY12" s="59" t="s">
+        <v>65</v>
+      </c>
+      <c r="AZ12" s="5"/>
+      <c r="BA12" s="1"/>
+      <c r="BB12" s="1"/>
+      <c r="BC12" s="1"/>
+      <c r="BD12" s="6"/>
+      <c r="BE12" s="1"/>
+      <c r="BF12" s="59"/>
+      <c r="BG12" s="1"/>
+      <c r="BH12" s="1"/>
+      <c r="BI12" s="1"/>
+    </row>
+    <row r="13" spans="2:61" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="1"/>
       <c r="C13" s="6">
         <v>3</v>
@@ -3989,10 +4119,25 @@
       <c r="AT13" s="1"/>
       <c r="AU13" s="1"/>
       <c r="AV13" s="1"/>
-      <c r="AW13" s="1"/>
+      <c r="AW13" s="6">
+        <v>3</v>
+      </c>
       <c r="AX13" s="1"/>
-    </row>
-    <row r="14" spans="2:50" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AY13" s="1"/>
+      <c r="AZ13" s="4"/>
+      <c r="BA13" s="1"/>
+      <c r="BB13" s="1"/>
+      <c r="BC13" s="1"/>
+      <c r="BD13" s="6">
+        <v>3</v>
+      </c>
+      <c r="BE13" s="1"/>
+      <c r="BF13" s="1"/>
+      <c r="BG13" s="1"/>
+      <c r="BH13" s="1"/>
+      <c r="BI13" s="1"/>
+    </row>
+    <row r="14" spans="2:61" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="1"/>
       <c r="C14" s="66" t="s">
         <v>61</v>
@@ -4056,10 +4201,25 @@
       <c r="AT14" s="1"/>
       <c r="AU14" s="1"/>
       <c r="AV14" s="1"/>
-      <c r="AW14" s="1"/>
+      <c r="AW14" s="66" t="s">
+        <v>61</v>
+      </c>
       <c r="AX14" s="1"/>
-    </row>
-    <row r="15" spans="2:50" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AY14" s="1"/>
+      <c r="AZ14" s="5"/>
+      <c r="BA14" s="1"/>
+      <c r="BB14" s="1"/>
+      <c r="BC14" s="1"/>
+      <c r="BD14" s="66" t="s">
+        <v>61</v>
+      </c>
+      <c r="BE14" s="1"/>
+      <c r="BF14" s="1"/>
+      <c r="BG14" s="1"/>
+      <c r="BH14" s="1"/>
+      <c r="BI14" s="1"/>
+    </row>
+    <row r="15" spans="2:61" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="1"/>
       <c r="C15" s="8">
         <v>6</v>
@@ -4123,10 +4283,25 @@
       <c r="AT15" s="1"/>
       <c r="AU15" s="1"/>
       <c r="AV15" s="1"/>
-      <c r="AW15" s="1"/>
-      <c r="AX15" s="1"/>
-    </row>
-    <row r="16" spans="2:50" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AW15" s="8">
+        <v>6</v>
+      </c>
+      <c r="AX15" s="4"/>
+      <c r="AY15" s="5"/>
+      <c r="AZ15" s="5"/>
+      <c r="BA15" s="1"/>
+      <c r="BB15" s="1"/>
+      <c r="BC15" s="1"/>
+      <c r="BD15" s="8">
+        <v>6</v>
+      </c>
+      <c r="BE15" s="4"/>
+      <c r="BF15" s="5"/>
+      <c r="BG15" s="1"/>
+      <c r="BH15" s="1"/>
+      <c r="BI15" s="1"/>
+    </row>
+    <row r="16" spans="2:61" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="1"/>
       <c r="C16" s="6"/>
       <c r="D16" s="59" t="s">
@@ -4190,10 +4365,25 @@
       <c r="AT16" s="1"/>
       <c r="AU16" s="1"/>
       <c r="AV16" s="1"/>
-      <c r="AW16" s="1"/>
-      <c r="AX16" s="1"/>
-    </row>
-    <row r="17" spans="2:50" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AW16" s="6"/>
+      <c r="AX16" s="59" t="s">
+        <v>64</v>
+      </c>
+      <c r="AY16" s="5"/>
+      <c r="AZ16" s="5"/>
+      <c r="BA16" s="1"/>
+      <c r="BB16" s="1"/>
+      <c r="BC16" s="1"/>
+      <c r="BD16" s="6"/>
+      <c r="BE16" s="59" t="s">
+        <v>64</v>
+      </c>
+      <c r="BF16" s="5"/>
+      <c r="BG16" s="1"/>
+      <c r="BH16" s="1"/>
+      <c r="BI16" s="1"/>
+    </row>
+    <row r="17" spans="2:61" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="1"/>
       <c r="C17" s="6">
         <v>2</v>
@@ -4257,10 +4447,25 @@
       <c r="AT17" s="1"/>
       <c r="AU17" s="1"/>
       <c r="AV17" s="1"/>
-      <c r="AW17" s="1"/>
+      <c r="AW17" s="6">
+        <v>2</v>
+      </c>
       <c r="AX17" s="1"/>
-    </row>
-    <row r="18" spans="2:50" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AY17" s="4"/>
+      <c r="AZ17" s="1"/>
+      <c r="BA17" s="1"/>
+      <c r="BB17" s="1"/>
+      <c r="BC17" s="1"/>
+      <c r="BD17" s="6">
+        <v>2</v>
+      </c>
+      <c r="BE17" s="1"/>
+      <c r="BF17" s="4"/>
+      <c r="BG17" s="1"/>
+      <c r="BH17" s="1"/>
+      <c r="BI17" s="1"/>
+    </row>
+    <row r="18" spans="2:61" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="1"/>
       <c r="C18" s="66" t="s">
         <v>62</v>
@@ -4328,10 +4533,25 @@
       <c r="AT18" s="1"/>
       <c r="AU18" s="1"/>
       <c r="AV18" s="1"/>
-      <c r="AW18" s="1"/>
+      <c r="AW18" s="66" t="s">
+        <v>62</v>
+      </c>
       <c r="AX18" s="1"/>
-    </row>
-    <row r="19" spans="2:50" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AY18" s="5"/>
+      <c r="AZ18" s="1"/>
+      <c r="BA18" s="1"/>
+      <c r="BB18" s="1"/>
+      <c r="BC18" s="1"/>
+      <c r="BD18" s="66" t="s">
+        <v>62</v>
+      </c>
+      <c r="BE18" s="1"/>
+      <c r="BF18" s="5"/>
+      <c r="BG18" s="1"/>
+      <c r="BH18" s="1"/>
+      <c r="BI18" s="1"/>
+    </row>
+    <row r="19" spans="2:61" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="1"/>
       <c r="C19" s="8">
         <v>7</v>
@@ -4399,10 +4619,29 @@
       </c>
       <c r="AU19" s="1"/>
       <c r="AV19" s="1"/>
-      <c r="AW19" s="1"/>
-      <c r="AX19" s="1"/>
-    </row>
-    <row r="20" spans="2:50" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AW19" s="8">
+        <v>7</v>
+      </c>
+      <c r="AX19" s="4"/>
+      <c r="AY19" s="1"/>
+      <c r="AZ19" s="1"/>
+      <c r="BA19" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="BB19" s="1"/>
+      <c r="BC19" s="1"/>
+      <c r="BD19" s="8">
+        <v>7</v>
+      </c>
+      <c r="BE19" s="4"/>
+      <c r="BF19" s="1"/>
+      <c r="BG19" s="1"/>
+      <c r="BH19" s="83" t="s">
+        <v>65</v>
+      </c>
+      <c r="BI19" s="83"/>
+    </row>
+    <row r="20" spans="2:61" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -4470,8 +4709,23 @@
       <c r="AV20" s="1"/>
       <c r="AW20" s="1"/>
       <c r="AX20" s="1"/>
-    </row>
-    <row r="21" spans="2:50" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AY20" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AZ20" s="1"/>
+      <c r="BA20" s="66"/>
+      <c r="BB20" s="5"/>
+      <c r="BC20" s="1"/>
+      <c r="BD20" s="1"/>
+      <c r="BE20" s="1"/>
+      <c r="BF20" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="BG20" s="1"/>
+      <c r="BH20" s="84"/>
+      <c r="BI20" s="83"/>
+    </row>
+    <row r="21" spans="2:61" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
@@ -4544,9 +4798,32 @@
       <c r="AU21" s="5"/>
       <c r="AV21" s="1"/>
       <c r="AW21" s="1"/>
-      <c r="AX21" s="1"/>
-    </row>
-    <row r="22" spans="2:50" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AX21" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="AY21" s="66" t="s">
+        <v>81</v>
+      </c>
+      <c r="AZ21" s="1"/>
+      <c r="BA21" s="59" t="s">
+        <v>115</v>
+      </c>
+      <c r="BB21" s="5"/>
+      <c r="BC21" s="1"/>
+      <c r="BD21" s="1"/>
+      <c r="BE21" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="BF21" s="66" t="s">
+        <v>81</v>
+      </c>
+      <c r="BG21" s="1"/>
+      <c r="BH21" s="84" t="s">
+        <v>115</v>
+      </c>
+      <c r="BI21" s="83"/>
+    </row>
+    <row r="22" spans="2:61" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
@@ -4611,9 +4888,24 @@
       <c r="AU22" s="4"/>
       <c r="AV22" s="1"/>
       <c r="AW22" s="1"/>
-      <c r="AX22" s="1"/>
-    </row>
-    <row r="23" spans="2:50" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AX22" s="66" t="s">
+        <v>66</v>
+      </c>
+      <c r="AY22" s="8"/>
+      <c r="AZ22" s="4"/>
+      <c r="BA22" s="5"/>
+      <c r="BB22" s="4"/>
+      <c r="BC22" s="1"/>
+      <c r="BD22" s="1"/>
+      <c r="BE22" s="66" t="s">
+        <v>66</v>
+      </c>
+      <c r="BF22" s="8"/>
+      <c r="BG22" s="4"/>
+      <c r="BH22" s="83"/>
+      <c r="BI22" s="83"/>
+    </row>
+    <row r="23" spans="2:61" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -4674,9 +4966,26 @@
       <c r="AU23" s="5"/>
       <c r="AV23" s="1"/>
       <c r="AW23" s="1"/>
-      <c r="AX23" s="1"/>
-    </row>
-    <row r="24" spans="2:50" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AX23" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="AY23" s="4"/>
+      <c r="AZ23" s="59" t="s">
+        <v>90</v>
+      </c>
+      <c r="BA23" s="5"/>
+      <c r="BB23" s="5"/>
+      <c r="BC23" s="1"/>
+      <c r="BD23" s="1"/>
+      <c r="BE23" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="BF23" s="4"/>
+      <c r="BG23" s="59"/>
+      <c r="BH23" s="83"/>
+      <c r="BI23" s="83"/>
+    </row>
+    <row r="24" spans="2:61" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
@@ -4732,8 +5041,23 @@
       <c r="AV24" s="1"/>
       <c r="AW24" s="1"/>
       <c r="AX24" s="1"/>
-    </row>
-    <row r="25" spans="2:50" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AY24" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="AZ24" s="1"/>
+      <c r="BA24" s="4"/>
+      <c r="BB24" s="1"/>
+      <c r="BC24" s="1"/>
+      <c r="BD24" s="1"/>
+      <c r="BE24" s="1"/>
+      <c r="BF24" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="BG24" s="1"/>
+      <c r="BH24" s="83"/>
+      <c r="BI24" s="83"/>
+    </row>
+    <row r="25" spans="2:61" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
@@ -4792,9 +5116,28 @@
       <c r="AU25" s="1"/>
       <c r="AV25" s="1"/>
       <c r="AW25" s="1"/>
-      <c r="AX25" s="1"/>
-    </row>
-    <row r="26" spans="2:50" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AX25" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="AY25" s="66" t="s">
+        <v>91</v>
+      </c>
+      <c r="AZ25" s="1"/>
+      <c r="BA25" s="5"/>
+      <c r="BB25" s="1"/>
+      <c r="BC25" s="1"/>
+      <c r="BD25" s="1"/>
+      <c r="BE25" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="BF25" s="66" t="s">
+        <v>91</v>
+      </c>
+      <c r="BG25" s="1"/>
+      <c r="BH25" s="83"/>
+      <c r="BI25" s="83"/>
+    </row>
+    <row r="26" spans="2:61" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
@@ -4849,9 +5192,24 @@
       <c r="AU26" s="1"/>
       <c r="AV26" s="1"/>
       <c r="AW26" s="1"/>
-      <c r="AX26" s="1"/>
-    </row>
-    <row r="27" spans="2:50" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AX26" s="66" t="s">
+        <v>92</v>
+      </c>
+      <c r="AY26" s="8"/>
+      <c r="AZ26" s="4"/>
+      <c r="BA26" s="1"/>
+      <c r="BB26" s="1"/>
+      <c r="BC26" s="1"/>
+      <c r="BD26" s="1"/>
+      <c r="BE26" s="66" t="s">
+        <v>92</v>
+      </c>
+      <c r="BF26" s="8"/>
+      <c r="BG26" s="4"/>
+      <c r="BH26" s="1"/>
+      <c r="BI26" s="1"/>
+    </row>
+    <row r="27" spans="2:61" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
@@ -4904,9 +5262,24 @@
       <c r="AU27" s="1"/>
       <c r="AV27" s="1"/>
       <c r="AW27" s="1"/>
-      <c r="AX27" s="1"/>
-    </row>
-    <row r="28" spans="2:50" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="AX27" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="AY27" s="4"/>
+      <c r="AZ27" s="1"/>
+      <c r="BA27" s="1"/>
+      <c r="BB27" s="1"/>
+      <c r="BC27" s="1"/>
+      <c r="BD27" s="1"/>
+      <c r="BE27" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="BF27" s="4"/>
+      <c r="BG27" s="1"/>
+      <c r="BH27" s="1"/>
+      <c r="BI27" s="1"/>
+    </row>
+    <row r="28" spans="2:61" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
@@ -4956,6 +5329,17 @@
       <c r="AV28" s="1"/>
       <c r="AW28" s="1"/>
       <c r="AX28" s="1"/>
+      <c r="AY28" s="1"/>
+      <c r="AZ28" s="1"/>
+      <c r="BA28" s="1"/>
+      <c r="BB28" s="1"/>
+      <c r="BC28" s="1"/>
+      <c r="BD28" s="1"/>
+      <c r="BE28" s="1"/>
+      <c r="BF28" s="1"/>
+      <c r="BG28" s="1"/>
+      <c r="BH28" s="1"/>
+      <c r="BI28" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6427,8 +6811,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D84D55B-86DB-41A7-86B6-8D3E6C4FEE99}">
   <dimension ref="C4:J29"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22:G28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14:H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7325,7 +7709,7 @@
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
-      <c r="H21" s="83"/>
+      <c r="H21" s="6"/>
       <c r="I21" s="7"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
@@ -7344,7 +7728,7 @@
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
-      <c r="H22" s="83"/>
+      <c r="H22" s="6"/>
       <c r="I22" s="1" t="s">
         <v>110</v>
       </c>
@@ -7363,7 +7747,7 @@
       <c r="E23" s="4"/>
       <c r="F23" s="5"/>
       <c r="G23" s="1"/>
-      <c r="H23" s="83"/>
+      <c r="H23" s="6"/>
       <c r="I23" s="9"/>
       <c r="J23" s="1"/>
       <c r="K23" s="5"/>
@@ -11525,32 +11909,32 @@
       <c r="I9" s="5"/>
     </row>
     <row r="10" spans="2:9" ht="4.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="77" t="s">
+      <c r="B10" s="76" t="s">
         <v>25</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="79"/>
-      <c r="F10" s="80"/>
+      <c r="E10" s="80"/>
+      <c r="F10" s="75"/>
       <c r="G10" s="6"/>
       <c r="H10" s="1"/>
       <c r="I10" s="5"/>
     </row>
     <row r="11" spans="2:9" ht="4.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="77"/>
+      <c r="B11" s="76"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="79"/>
-      <c r="F11" s="80"/>
+      <c r="E11" s="80"/>
+      <c r="F11" s="75"/>
       <c r="G11" s="6"/>
       <c r="H11" s="1"/>
       <c r="I11" s="5"/>
     </row>
     <row r="12" spans="2:9" ht="4.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="78"/>
+      <c r="B12" s="77"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="80"/>
+      <c r="E12" s="75"/>
       <c r="F12" s="1"/>
       <c r="G12" s="6"/>
       <c r="H12" s="1"/>
@@ -11558,37 +11942,37 @@
     </row>
     <row r="13" spans="2:9" ht="4.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B13" s="2"/>
-      <c r="C13" s="77" t="s">
+      <c r="C13" s="76" t="s">
         <v>29</v>
       </c>
       <c r="D13" s="1"/>
-      <c r="E13" s="80"/>
+      <c r="E13" s="75"/>
       <c r="F13" s="1"/>
       <c r="G13" s="6"/>
       <c r="H13" s="1"/>
-      <c r="I13" s="75" t="s">
+      <c r="I13" s="78" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="14" spans="2:9" ht="4.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="14"/>
-      <c r="C14" s="77"/>
-      <c r="D14" s="80"/>
-      <c r="E14" s="79"/>
+      <c r="C14" s="76"/>
+      <c r="D14" s="75"/>
+      <c r="E14" s="80"/>
       <c r="F14" s="1"/>
       <c r="G14" s="6"/>
       <c r="H14" s="1"/>
-      <c r="I14" s="75"/>
+      <c r="I14" s="78"/>
     </row>
     <row r="15" spans="2:9" ht="4.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="18"/>
-      <c r="C15" s="78"/>
-      <c r="D15" s="80"/>
-      <c r="E15" s="79"/>
+      <c r="C15" s="77"/>
+      <c r="D15" s="75"/>
+      <c r="E15" s="80"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
-      <c r="I15" s="76"/>
+      <c r="I15" s="79"/>
     </row>
     <row r="16" spans="2:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="8" t="s">
@@ -11676,17 +12060,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="I13:I15"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="E14:E15"/>
     <mergeCell ref="D20:F21"/>
     <mergeCell ref="F16:F17"/>
     <mergeCell ref="F10:F11"/>
     <mergeCell ref="C13:C15"/>
     <mergeCell ref="D14:D15"/>
     <mergeCell ref="E12:E13"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="I13:I15"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="E14:E15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>